<commit_message>
first 100 abstracts done
</commit_message>
<xml_diff>
--- a/abstracts.xlsx
+++ b/abstracts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myharrisburgu-my.sharepoint.com/personal/ebuchanan_harrisburgu_edu/Documents/Research/2 projects/LAB2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac924\Documents\GitHub\LAB2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{237257E3-1004-5440-B853-6D2D5DF70C77}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92638ED8-EF0A-4CCD-984F-548DE707A054}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{52E4A73F-0506-324F-90E4-F45C75E5528B}"/>
+    <workbookView xWindow="375" yWindow="465" windowWidth="28035" windowHeight="17040" xr2:uid="{52E4A73F-0506-324F-90E4-F45C75E5528B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="888">
   <si>
     <t>Zettersten, A., &amp; Kučera, H. (1978). A word-frequency list based on American English press reportage. Retrieved from https://scholar.google.com/scholar?hl=en&amp;as_sdt=0%2C25&amp;q=A+word-frequency+list+based+on+American+English+press+reportage&amp;btnG=</t>
   </si>
@@ -31239,6 +31238,9 @@
   </si>
   <si>
     <t xml:space="preserve">citation </t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -31605,11 +31607,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0998DB5B-4846-834A-B712-19266A922CC0}">
   <dimension ref="A1:B886"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -31620,556 +31622,856 @@
       </c>
     </row>
     <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>885</v>
+      </c>
       <c r="B2" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>885</v>
+      </c>
       <c r="B3" t="s">
         <v>814</v>
       </c>
     </row>
     <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>885</v>
+      </c>
       <c r="B4" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>885</v>
+      </c>
       <c r="B5" t="s">
         <v>700</v>
       </c>
     </row>
     <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>887</v>
+      </c>
       <c r="B6" t="s">
         <v>784</v>
       </c>
     </row>
     <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>885</v>
+      </c>
       <c r="B7" t="s">
         <v>605</v>
       </c>
     </row>
     <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>885</v>
+      </c>
       <c r="B8" t="s">
         <v>611</v>
       </c>
     </row>
     <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>885</v>
+      </c>
       <c r="B9" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>885</v>
+      </c>
       <c r="B10" t="s">
         <v>867</v>
       </c>
     </row>
     <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>885</v>
+      </c>
       <c r="B11" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>885</v>
+      </c>
       <c r="B12" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>885</v>
+      </c>
       <c r="B13" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>887</v>
+      </c>
       <c r="B14" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>885</v>
+      </c>
       <c r="B15" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>885</v>
+      </c>
       <c r="B16" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>885</v>
+      </c>
       <c r="B17" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>885</v>
+      </c>
       <c r="B18" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>885</v>
+      </c>
       <c r="B19" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>885</v>
+      </c>
       <c r="B20" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="21" spans="2:2">
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>887</v>
+      </c>
       <c r="B21" t="s">
         <v>880</v>
       </c>
     </row>
-    <row r="22" spans="2:2">
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>885</v>
+      </c>
       <c r="B22" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="23" spans="2:2">
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>885</v>
+      </c>
       <c r="B23" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="24" spans="2:2">
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>885</v>
+      </c>
       <c r="B24" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="25" spans="2:2">
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>885</v>
+      </c>
       <c r="B25" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="2:2">
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>885</v>
+      </c>
       <c r="B26" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="2:2">
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>885</v>
+      </c>
       <c r="B27" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="28" spans="2:2">
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>885</v>
+      </c>
       <c r="B28" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="29" spans="2:2">
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>885</v>
+      </c>
       <c r="B29" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="2:2">
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>885</v>
+      </c>
       <c r="B30" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="31" spans="2:2">
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>885</v>
+      </c>
       <c r="B31" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="32" spans="2:2">
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>885</v>
+      </c>
       <c r="B32" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>885</v>
+      </c>
       <c r="B33" t="s">
         <v>823</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>885</v>
+      </c>
       <c r="B34" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="35" spans="2:2">
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>885</v>
+      </c>
       <c r="B35" t="s">
         <v>847</v>
       </c>
     </row>
-    <row r="36" spans="2:2">
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>885</v>
+      </c>
       <c r="B36" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="2:2">
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>885</v>
+      </c>
       <c r="B37" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="2:2">
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>885</v>
+      </c>
       <c r="B38" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="39" spans="2:2">
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>885</v>
+      </c>
       <c r="B39" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="2:2">
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>885</v>
+      </c>
       <c r="B40" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="41" spans="2:2">
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>887</v>
+      </c>
       <c r="B41" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="2:2">
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>885</v>
+      </c>
       <c r="B42" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="43" spans="2:2">
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>885</v>
+      </c>
       <c r="B43" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="44" spans="2:2">
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>887</v>
+      </c>
       <c r="B44" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="45" spans="2:2">
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>885</v>
+      </c>
       <c r="B45" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="2:2">
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>885</v>
+      </c>
       <c r="B46" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="47" spans="2:2">
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>885</v>
+      </c>
       <c r="B47" t="s">
         <v>678</v>
       </c>
     </row>
-    <row r="48" spans="2:2">
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>885</v>
+      </c>
       <c r="B48" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="49" spans="2:2">
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>885</v>
+      </c>
       <c r="B49" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="50" spans="2:2">
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>885</v>
+      </c>
       <c r="B50" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="51" spans="2:2">
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>885</v>
+      </c>
       <c r="B51" t="s">
         <v>767</v>
       </c>
     </row>
-    <row r="52" spans="2:2">
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>885</v>
+      </c>
       <c r="B52" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="53" spans="2:2">
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>885</v>
+      </c>
       <c r="B53" t="s">
         <v>799</v>
       </c>
     </row>
-    <row r="54" spans="2:2">
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>885</v>
+      </c>
       <c r="B54" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="55" spans="2:2">
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>885</v>
+      </c>
       <c r="B55" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="56" spans="2:2">
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>885</v>
+      </c>
       <c r="B56" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="57" spans="2:2">
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>885</v>
+      </c>
       <c r="B57" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="2:2">
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>885</v>
+      </c>
       <c r="B58" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="2:2">
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>885</v>
+      </c>
       <c r="B59" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="60" spans="2:2">
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>885</v>
+      </c>
       <c r="B60" t="s">
         <v>831</v>
       </c>
     </row>
-    <row r="61" spans="2:2">
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>885</v>
+      </c>
       <c r="B61" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="62" spans="2:2">
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>885</v>
+      </c>
       <c r="B62" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="63" spans="2:2">
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>885</v>
+      </c>
       <c r="B63" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="64" spans="2:2">
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>885</v>
+      </c>
       <c r="B64" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="65" spans="2:2">
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>885</v>
+      </c>
       <c r="B65" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="66" spans="2:2">
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>885</v>
+      </c>
       <c r="B66" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="67" spans="2:2">
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>885</v>
+      </c>
       <c r="B67" t="s">
         <v>854</v>
       </c>
     </row>
-    <row r="68" spans="2:2">
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>885</v>
+      </c>
       <c r="B68" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="69" spans="2:2">
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>885</v>
+      </c>
       <c r="B69" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="70" spans="2:2">
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>885</v>
+      </c>
       <c r="B70" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="71" spans="2:2">
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>885</v>
+      </c>
       <c r="B71" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="72" spans="2:2">
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>885</v>
+      </c>
       <c r="B72" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="73" spans="2:2">
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>885</v>
+      </c>
       <c r="B73" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="74" spans="2:2">
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>885</v>
+      </c>
       <c r="B74" t="s">
         <v>715</v>
       </c>
     </row>
-    <row r="75" spans="2:2">
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>885</v>
+      </c>
       <c r="B75" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="76" spans="2:2">
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>885</v>
+      </c>
       <c r="B76" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="77" spans="2:2">
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>885</v>
+      </c>
       <c r="B77" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="78" spans="2:2">
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>887</v>
+      </c>
       <c r="B78" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="2:2">
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>885</v>
+      </c>
       <c r="B79" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="80" spans="2:2">
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>887</v>
+      </c>
       <c r="B80" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="81" spans="2:2">
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>885</v>
+      </c>
       <c r="B81" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="82" spans="2:2">
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>885</v>
+      </c>
       <c r="B82" t="s">
         <v>815</v>
       </c>
     </row>
-    <row r="83" spans="2:2">
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>885</v>
+      </c>
       <c r="B83" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="84" spans="2:2">
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>885</v>
+      </c>
       <c r="B84" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="85" spans="2:2">
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>885</v>
+      </c>
       <c r="B85" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="86" spans="2:2">
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>885</v>
+      </c>
       <c r="B86" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="87" spans="2:2">
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>885</v>
+      </c>
       <c r="B87" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="88" spans="2:2">
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>885</v>
+      </c>
       <c r="B88" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="89" spans="2:2">
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>885</v>
+      </c>
       <c r="B89" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="90" spans="2:2">
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>885</v>
+      </c>
       <c r="B90" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="91" spans="2:2">
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>885</v>
+      </c>
       <c r="B91" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="92" spans="2:2">
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>885</v>
+      </c>
       <c r="B92" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="93" spans="2:2">
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>885</v>
+      </c>
       <c r="B93" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="94" spans="2:2">
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>885</v>
+      </c>
       <c r="B94" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="95" spans="2:2">
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>885</v>
+      </c>
       <c r="B95" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="96" spans="2:2">
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>885</v>
+      </c>
       <c r="B96" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="97" spans="2:2">
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>885</v>
+      </c>
       <c r="B97" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="98" spans="2:2">
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>885</v>
+      </c>
       <c r="B98" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="99" spans="2:2">
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>885</v>
+      </c>
       <c r="B99" t="s">
         <v>870</v>
       </c>
     </row>
-    <row r="100" spans="2:2">
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>885</v>
+      </c>
       <c r="B100" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="101" spans="2:2">
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>885</v>
+      </c>
       <c r="B101" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="102" spans="2:2">
+    <row r="102" spans="1:2">
       <c r="B102" t="s">
         <v>881</v>
       </c>
     </row>
-    <row r="103" spans="2:2">
+    <row r="103" spans="1:2">
       <c r="B103" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="104" spans="2:2">
+    <row r="104" spans="1:2">
       <c r="B104" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="105" spans="2:2">
+    <row r="105" spans="1:2">
       <c r="B105" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="106" spans="2:2">
+    <row r="106" spans="1:2">
       <c r="B106" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="107" spans="2:2">
+    <row r="107" spans="1:2">
       <c r="B107" t="s">
         <v>873</v>
       </c>
     </row>
-    <row r="108" spans="2:2">
+    <row r="108" spans="1:2">
       <c r="B108" t="s">
         <v>862</v>
       </c>
     </row>
-    <row r="109" spans="2:2">
+    <row r="109" spans="1:2">
       <c r="B109" t="s">
         <v>800</v>
       </c>
     </row>
-    <row r="110" spans="2:2">
+    <row r="110" spans="1:2">
       <c r="B110" t="s">
         <v>801</v>
       </c>
     </row>
-    <row r="111" spans="2:2">
+    <row r="111" spans="1:2">
       <c r="B111" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="112" spans="2:2">
+    <row r="112" spans="1:2">
       <c r="B112" t="s">
         <v>520</v>
       </c>

</xml_diff>

<commit_message>
about 1/3 of the way done with abstracts
</commit_message>
<xml_diff>
--- a/abstracts.xlsx
+++ b/abstracts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac924\Documents\GitHub\LAB2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92638ED8-EF0A-4CCD-984F-548DE707A054}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692F8B67-0909-45D5-8506-15C3A2E69099}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="375" yWindow="465" windowWidth="28035" windowHeight="17040" xr2:uid="{52E4A73F-0506-324F-90E4-F45C75E5528B}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="888">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1220" uniqueCount="888">
   <si>
     <t>Zettersten, A., &amp; Kučera, H. (1978). A word-frequency list based on American English press reportage. Retrieved from https://scholar.google.com/scholar?hl=en&amp;as_sdt=0%2C25&amp;q=A+word-frequency+list+based+on+American+English+press+reportage&amp;btnG=</t>
   </si>
@@ -31607,8 +31607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0998DB5B-4846-834A-B712-19266A922CC0}">
   <dimension ref="A1:B886"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="A325" workbookViewId="0">
+      <selection activeCell="A335" sqref="A335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
@@ -32422,1176 +32422,1875 @@
       </c>
     </row>
     <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>885</v>
+      </c>
       <c r="B102" t="s">
         <v>881</v>
       </c>
     </row>
     <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>887</v>
+      </c>
       <c r="B103" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>885</v>
+      </c>
       <c r="B104" t="s">
         <v>798</v>
       </c>
     </row>
     <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>885</v>
+      </c>
       <c r="B105" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>887</v>
+      </c>
       <c r="B106" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>885</v>
+      </c>
       <c r="B107" t="s">
         <v>873</v>
       </c>
     </row>
     <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>885</v>
+      </c>
       <c r="B108" t="s">
         <v>862</v>
       </c>
     </row>
     <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>885</v>
+      </c>
       <c r="B109" t="s">
         <v>800</v>
       </c>
     </row>
     <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>885</v>
+      </c>
       <c r="B110" t="s">
         <v>801</v>
       </c>
     </row>
     <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>885</v>
+      </c>
       <c r="B111" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>885</v>
+      </c>
       <c r="B112" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="113" spans="2:2">
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>885</v>
+      </c>
       <c r="B113" t="s">
         <v>802</v>
       </c>
     </row>
-    <row r="114" spans="2:2">
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>885</v>
+      </c>
       <c r="B114" t="s">
         <v>803</v>
       </c>
     </row>
-    <row r="115" spans="2:2">
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>885</v>
+      </c>
       <c r="B115" t="s">
         <v>820</v>
       </c>
     </row>
-    <row r="116" spans="2:2">
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>885</v>
+      </c>
       <c r="B116" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="117" spans="2:2">
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>885</v>
+      </c>
       <c r="B117" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="118" spans="2:2">
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>885</v>
+      </c>
       <c r="B118" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="119" spans="2:2">
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>885</v>
+      </c>
       <c r="B119" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="120" spans="2:2">
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>885</v>
+      </c>
       <c r="B120" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="121" spans="2:2">
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>885</v>
+      </c>
       <c r="B121" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="122" spans="2:2">
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>885</v>
+      </c>
       <c r="B122" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="123" spans="2:2">
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>885</v>
+      </c>
       <c r="B123" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="124" spans="2:2">
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>885</v>
+      </c>
       <c r="B124" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="125" spans="2:2">
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>885</v>
+      </c>
       <c r="B125" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="126" spans="2:2">
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>885</v>
+      </c>
       <c r="B126" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="127" spans="2:2">
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
+        <v>887</v>
+      </c>
       <c r="B127" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="128" spans="2:2">
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>885</v>
+      </c>
       <c r="B128" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="129" spans="2:2">
+    <row r="129" spans="1:2">
+      <c r="A129" t="s">
+        <v>885</v>
+      </c>
       <c r="B129" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="130" spans="2:2">
+    <row r="130" spans="1:2">
+      <c r="A130" t="s">
+        <v>885</v>
+      </c>
       <c r="B130" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="131" spans="2:2">
+    <row r="131" spans="1:2">
+      <c r="A131" t="s">
+        <v>885</v>
+      </c>
       <c r="B131" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="132" spans="2:2">
+    <row r="132" spans="1:2">
+      <c r="A132" t="s">
+        <v>885</v>
+      </c>
       <c r="B132" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="133" spans="2:2">
+    <row r="133" spans="1:2">
+      <c r="A133" t="s">
+        <v>885</v>
+      </c>
       <c r="B133" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="134" spans="2:2">
+    <row r="134" spans="1:2">
+      <c r="A134" t="s">
+        <v>885</v>
+      </c>
       <c r="B134" t="s">
         <v>748</v>
       </c>
     </row>
-    <row r="135" spans="2:2">
+    <row r="135" spans="1:2">
+      <c r="A135" t="s">
+        <v>885</v>
+      </c>
       <c r="B135" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="136" spans="2:2">
+    <row r="136" spans="1:2">
+      <c r="A136" t="s">
+        <v>885</v>
+      </c>
       <c r="B136" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="137" spans="2:2">
+    <row r="137" spans="1:2">
+      <c r="A137" t="s">
+        <v>885</v>
+      </c>
       <c r="B137" t="s">
         <v>804</v>
       </c>
     </row>
-    <row r="138" spans="2:2">
+    <row r="138" spans="1:2">
+      <c r="A138" t="s">
+        <v>885</v>
+      </c>
       <c r="B138" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="139" spans="2:2">
+    <row r="139" spans="1:2">
+      <c r="A139" t="s">
+        <v>885</v>
+      </c>
       <c r="B139" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="140" spans="2:2">
+    <row r="140" spans="1:2">
+      <c r="A140" t="s">
+        <v>885</v>
+      </c>
       <c r="B140" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="141" spans="2:2">
+    <row r="141" spans="1:2">
+      <c r="A141" t="s">
+        <v>885</v>
+      </c>
       <c r="B141" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="142" spans="2:2">
+    <row r="142" spans="1:2">
+      <c r="A142" t="s">
+        <v>885</v>
+      </c>
       <c r="B142" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="143" spans="2:2">
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
+        <v>885</v>
+      </c>
       <c r="B143" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="144" spans="2:2">
+    <row r="144" spans="1:2">
+      <c r="A144" t="s">
+        <v>885</v>
+      </c>
       <c r="B144" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="145" spans="2:2">
+    <row r="145" spans="1:2">
+      <c r="A145" t="s">
+        <v>885</v>
+      </c>
       <c r="B145" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="146" spans="2:2">
+    <row r="146" spans="1:2">
+      <c r="A146" t="s">
+        <v>885</v>
+      </c>
       <c r="B146" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="147" spans="2:2">
+    <row r="147" spans="1:2">
+      <c r="A147" t="s">
+        <v>885</v>
+      </c>
       <c r="B147" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="148" spans="2:2">
+    <row r="148" spans="1:2">
+      <c r="A148" t="s">
+        <v>885</v>
+      </c>
       <c r="B148" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="149" spans="2:2">
+    <row r="149" spans="1:2">
+      <c r="A149" t="s">
+        <v>887</v>
+      </c>
       <c r="B149" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="150" spans="2:2">
+    <row r="150" spans="1:2">
+      <c r="A150" t="s">
+        <v>885</v>
+      </c>
       <c r="B150" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="151" spans="2:2">
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
+        <v>885</v>
+      </c>
       <c r="B151" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="152" spans="2:2">
+    <row r="152" spans="1:2">
+      <c r="A152" t="s">
+        <v>887</v>
+      </c>
       <c r="B152" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="153" spans="2:2">
+    <row r="153" spans="1:2">
+      <c r="A153" t="s">
+        <v>885</v>
+      </c>
       <c r="B153" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="154" spans="2:2">
+    <row r="154" spans="1:2">
+      <c r="A154" t="s">
+        <v>885</v>
+      </c>
       <c r="B154" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="155" spans="2:2">
+    <row r="155" spans="1:2">
+      <c r="A155" t="s">
+        <v>887</v>
+      </c>
       <c r="B155" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="156" spans="2:2">
+    <row r="156" spans="1:2">
+      <c r="A156" t="s">
+        <v>885</v>
+      </c>
       <c r="B156" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="157" spans="2:2">
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>885</v>
+      </c>
       <c r="B157" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="158" spans="2:2">
+    <row r="158" spans="1:2">
+      <c r="A158" t="s">
+        <v>885</v>
+      </c>
       <c r="B158" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="159" spans="2:2">
+    <row r="159" spans="1:2">
+      <c r="A159" t="s">
+        <v>885</v>
+      </c>
       <c r="B159" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="160" spans="2:2">
+    <row r="160" spans="1:2">
+      <c r="A160" t="s">
+        <v>887</v>
+      </c>
       <c r="B160" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="161" spans="2:2">
+    <row r="161" spans="1:2">
+      <c r="A161" t="s">
+        <v>885</v>
+      </c>
       <c r="B161" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="162" spans="2:2">
+    <row r="162" spans="1:2">
+      <c r="A162" t="s">
+        <v>885</v>
+      </c>
       <c r="B162" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="163" spans="2:2">
+    <row r="163" spans="1:2">
+      <c r="A163" t="s">
+        <v>885</v>
+      </c>
       <c r="B163" t="s">
         <v>760</v>
       </c>
     </row>
-    <row r="164" spans="2:2">
+    <row r="164" spans="1:2">
+      <c r="A164" t="s">
+        <v>885</v>
+      </c>
       <c r="B164" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="165" spans="2:2">
+    <row r="165" spans="1:2">
+      <c r="A165" t="s">
+        <v>885</v>
+      </c>
       <c r="B165" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="166" spans="2:2">
+    <row r="166" spans="1:2">
+      <c r="A166" t="s">
+        <v>885</v>
+      </c>
       <c r="B166" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="167" spans="2:2">
+    <row r="167" spans="1:2">
+      <c r="A167" t="s">
+        <v>885</v>
+      </c>
       <c r="B167" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="168" spans="2:2">
+    <row r="168" spans="1:2">
+      <c r="A168" t="s">
+        <v>885</v>
+      </c>
       <c r="B168" t="s">
         <v>725</v>
       </c>
     </row>
-    <row r="169" spans="2:2">
+    <row r="169" spans="1:2">
+      <c r="A169" t="s">
+        <v>885</v>
+      </c>
       <c r="B169" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="170" spans="2:2">
+    <row r="170" spans="1:2">
+      <c r="A170" t="s">
+        <v>885</v>
+      </c>
       <c r="B170" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="171" spans="2:2">
+    <row r="171" spans="1:2">
+      <c r="A171" t="s">
+        <v>887</v>
+      </c>
       <c r="B171" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="172" spans="2:2">
+    <row r="172" spans="1:2">
+      <c r="A172" t="s">
+        <v>885</v>
+      </c>
       <c r="B172" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="173" spans="2:2">
+    <row r="173" spans="1:2">
+      <c r="A173" t="s">
+        <v>885</v>
+      </c>
       <c r="B173" t="s">
         <v>879</v>
       </c>
     </row>
-    <row r="174" spans="2:2">
+    <row r="174" spans="1:2">
+      <c r="A174" t="s">
+        <v>885</v>
+      </c>
       <c r="B174" t="s">
         <v>855</v>
       </c>
     </row>
-    <row r="175" spans="2:2">
+    <row r="175" spans="1:2">
+      <c r="A175" t="s">
+        <v>885</v>
+      </c>
       <c r="B175" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="176" spans="2:2">
+    <row r="176" spans="1:2">
+      <c r="A176" t="s">
+        <v>885</v>
+      </c>
       <c r="B176" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="177" spans="2:2">
+    <row r="177" spans="1:2">
+      <c r="A177" t="s">
+        <v>885</v>
+      </c>
       <c r="B177" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="178" spans="2:2">
+    <row r="178" spans="1:2">
+      <c r="A178" t="s">
+        <v>887</v>
+      </c>
       <c r="B178" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="179" spans="2:2">
+    <row r="179" spans="1:2">
+      <c r="A179" t="s">
+        <v>885</v>
+      </c>
       <c r="B179" t="s">
         <v>743</v>
       </c>
     </row>
-    <row r="180" spans="2:2">
+    <row r="180" spans="1:2">
+      <c r="A180" t="s">
+        <v>885</v>
+      </c>
       <c r="B180" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="181" spans="2:2">
+    <row r="181" spans="1:2">
+      <c r="A181" t="s">
+        <v>885</v>
+      </c>
       <c r="B181" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="182" spans="2:2">
+    <row r="182" spans="1:2">
+      <c r="A182" t="s">
+        <v>885</v>
+      </c>
       <c r="B182" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="183" spans="2:2">
+    <row r="183" spans="1:2">
+      <c r="A183" t="s">
+        <v>885</v>
+      </c>
       <c r="B183" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="184" spans="2:2">
+    <row r="184" spans="1:2">
+      <c r="A184" t="s">
+        <v>885</v>
+      </c>
       <c r="B184" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="185" spans="2:2">
+    <row r="185" spans="1:2">
+      <c r="A185" t="s">
+        <v>885</v>
+      </c>
       <c r="B185" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="186" spans="2:2">
+    <row r="186" spans="1:2">
+      <c r="A186" t="s">
+        <v>885</v>
+      </c>
       <c r="B186" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="187" spans="2:2">
+    <row r="187" spans="1:2">
+      <c r="A187" t="s">
+        <v>885</v>
+      </c>
       <c r="B187" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="188" spans="2:2">
+    <row r="188" spans="1:2">
+      <c r="A188" t="s">
+        <v>885</v>
+      </c>
       <c r="B188" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="189" spans="2:2">
+    <row r="189" spans="1:2">
+      <c r="A189" t="s">
+        <v>885</v>
+      </c>
       <c r="B189" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="190" spans="2:2">
+    <row r="190" spans="1:2">
+      <c r="A190" t="s">
+        <v>885</v>
+      </c>
       <c r="B190" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="191" spans="2:2">
+    <row r="191" spans="1:2">
+      <c r="A191" t="s">
+        <v>885</v>
+      </c>
       <c r="B191" t="s">
         <v>775</v>
       </c>
     </row>
-    <row r="192" spans="2:2">
+    <row r="192" spans="1:2">
+      <c r="A192" t="s">
+        <v>885</v>
+      </c>
       <c r="B192" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="193" spans="2:2">
+    <row r="193" spans="1:2">
+      <c r="A193" t="s">
+        <v>887</v>
+      </c>
       <c r="B193" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="194" spans="2:2">
+    <row r="194" spans="1:2">
+      <c r="A194" t="s">
+        <v>885</v>
+      </c>
       <c r="B194" t="s">
         <v>805</v>
       </c>
     </row>
-    <row r="195" spans="2:2">
+    <row r="195" spans="1:2">
+      <c r="A195" t="s">
+        <v>885</v>
+      </c>
       <c r="B195" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="196" spans="2:2">
+    <row r="196" spans="1:2">
+      <c r="A196" t="s">
+        <v>885</v>
+      </c>
       <c r="B196" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="197" spans="2:2">
+    <row r="197" spans="1:2">
+      <c r="A197" t="s">
+        <v>885</v>
+      </c>
       <c r="B197" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="198" spans="2:2">
+    <row r="198" spans="1:2">
+      <c r="A198" t="s">
+        <v>885</v>
+      </c>
       <c r="B198" t="s">
         <v>818</v>
       </c>
     </row>
-    <row r="199" spans="2:2">
+    <row r="199" spans="1:2">
+      <c r="A199" t="s">
+        <v>885</v>
+      </c>
       <c r="B199" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="200" spans="2:2">
+    <row r="200" spans="1:2">
+      <c r="A200" t="s">
+        <v>885</v>
+      </c>
       <c r="B200" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="201" spans="2:2">
+    <row r="201" spans="1:2">
+      <c r="A201" t="s">
+        <v>885</v>
+      </c>
       <c r="B201" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="202" spans="2:2">
+    <row r="202" spans="1:2">
+      <c r="A202" t="s">
+        <v>887</v>
+      </c>
       <c r="B202" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="203" spans="2:2">
+    <row r="203" spans="1:2">
+      <c r="A203" t="s">
+        <v>885</v>
+      </c>
       <c r="B203" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="204" spans="2:2">
+    <row r="204" spans="1:2">
+      <c r="A204" t="s">
+        <v>885</v>
+      </c>
       <c r="B204" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="205" spans="2:2">
+    <row r="205" spans="1:2">
+      <c r="A205" t="s">
+        <v>885</v>
+      </c>
       <c r="B205" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="206" spans="2:2">
+    <row r="206" spans="1:2">
+      <c r="A206" t="s">
+        <v>885</v>
+      </c>
       <c r="B206" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="207" spans="2:2">
+    <row r="207" spans="1:2">
+      <c r="A207" t="s">
+        <v>887</v>
+      </c>
       <c r="B207" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="208" spans="2:2">
+    <row r="208" spans="1:2">
+      <c r="A208" t="s">
+        <v>885</v>
+      </c>
       <c r="B208" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="209" spans="2:2">
+    <row r="209" spans="1:2">
+      <c r="A209" t="s">
+        <v>887</v>
+      </c>
       <c r="B209" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="210" spans="2:2">
+    <row r="210" spans="1:2">
+      <c r="A210" t="s">
+        <v>885</v>
+      </c>
       <c r="B210" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="211" spans="2:2">
+    <row r="211" spans="1:2">
+      <c r="A211" t="s">
+        <v>885</v>
+      </c>
       <c r="B211" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="212" spans="2:2">
+    <row r="212" spans="1:2">
+      <c r="A212" t="s">
+        <v>885</v>
+      </c>
       <c r="B212" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="213" spans="2:2">
+    <row r="213" spans="1:2">
+      <c r="A213" t="s">
+        <v>885</v>
+      </c>
       <c r="B213" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="214" spans="2:2">
+    <row r="214" spans="1:2">
+      <c r="A214" t="s">
+        <v>885</v>
+      </c>
       <c r="B214" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="215" spans="2:2">
+    <row r="215" spans="1:2">
+      <c r="A215" t="s">
+        <v>885</v>
+      </c>
       <c r="B215" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="216" spans="2:2">
+    <row r="216" spans="1:2">
+      <c r="A216" t="s">
+        <v>885</v>
+      </c>
       <c r="B216" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="217" spans="2:2">
+    <row r="217" spans="1:2">
+      <c r="A217" t="s">
+        <v>885</v>
+      </c>
       <c r="B217" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="218" spans="2:2">
+    <row r="218" spans="1:2">
+      <c r="A218" t="s">
+        <v>885</v>
+      </c>
       <c r="B218" t="s">
         <v>868</v>
       </c>
     </row>
-    <row r="219" spans="2:2">
+    <row r="219" spans="1:2">
+      <c r="A219" t="s">
+        <v>885</v>
+      </c>
       <c r="B219" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="220" spans="2:2">
+    <row r="220" spans="1:2">
+      <c r="A220" t="s">
+        <v>885</v>
+      </c>
       <c r="B220" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="221" spans="2:2">
+    <row r="221" spans="1:2">
+      <c r="A221" t="s">
+        <v>885</v>
+      </c>
       <c r="B221" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="222" spans="2:2">
+    <row r="222" spans="1:2">
+      <c r="A222" t="s">
+        <v>885</v>
+      </c>
       <c r="B222" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="223" spans="2:2">
+    <row r="223" spans="1:2">
+      <c r="A223" t="s">
+        <v>885</v>
+      </c>
       <c r="B223" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="224" spans="2:2">
+    <row r="224" spans="1:2">
+      <c r="A224" t="s">
+        <v>885</v>
+      </c>
       <c r="B224" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="225" spans="2:2">
+    <row r="225" spans="1:2">
+      <c r="A225" t="s">
+        <v>887</v>
+      </c>
       <c r="B225" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="226" spans="2:2">
+    <row r="226" spans="1:2">
+      <c r="A226" t="s">
+        <v>885</v>
+      </c>
       <c r="B226" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="227" spans="2:2">
+    <row r="227" spans="1:2">
+      <c r="A227" t="s">
+        <v>885</v>
+      </c>
       <c r="B227" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="228" spans="2:2">
+    <row r="228" spans="1:2">
+      <c r="A228" t="s">
+        <v>885</v>
+      </c>
       <c r="B228" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="229" spans="2:2">
+    <row r="229" spans="1:2">
+      <c r="A229" t="s">
+        <v>885</v>
+      </c>
       <c r="B229" t="s">
         <v>869</v>
       </c>
     </row>
-    <row r="230" spans="2:2">
+    <row r="230" spans="1:2">
+      <c r="A230" t="s">
+        <v>885</v>
+      </c>
       <c r="B230" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="231" spans="2:2">
+    <row r="231" spans="1:2">
+      <c r="A231" t="s">
+        <v>885</v>
+      </c>
       <c r="B231" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="232" spans="2:2">
+    <row r="232" spans="1:2">
+      <c r="A232" t="s">
+        <v>885</v>
+      </c>
       <c r="B232" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="233" spans="2:2">
+    <row r="233" spans="1:2">
+      <c r="A233" t="s">
+        <v>887</v>
+      </c>
       <c r="B233" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="234" spans="2:2">
+    <row r="234" spans="1:2">
+      <c r="A234" t="s">
+        <v>885</v>
+      </c>
       <c r="B234" t="s">
         <v>876</v>
       </c>
     </row>
-    <row r="235" spans="2:2">
+    <row r="235" spans="1:2">
+      <c r="A235" t="s">
+        <v>887</v>
+      </c>
       <c r="B235" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="236" spans="2:2">
+    <row r="236" spans="1:2">
+      <c r="A236" t="s">
+        <v>885</v>
+      </c>
       <c r="B236" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="237" spans="2:2">
+    <row r="237" spans="1:2">
+      <c r="A237" t="s">
+        <v>885</v>
+      </c>
       <c r="B237" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="238" spans="2:2">
+    <row r="238" spans="1:2">
+      <c r="A238" t="s">
+        <v>885</v>
+      </c>
       <c r="B238" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="239" spans="2:2">
+    <row r="239" spans="1:2">
+      <c r="A239" t="s">
+        <v>885</v>
+      </c>
       <c r="B239" t="s">
         <v>806</v>
       </c>
     </row>
-    <row r="240" spans="2:2">
+    <row r="240" spans="1:2">
+      <c r="A240" t="s">
+        <v>887</v>
+      </c>
       <c r="B240" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="241" spans="2:2">
+    <row r="241" spans="1:2">
+      <c r="A241" t="s">
+        <v>885</v>
+      </c>
       <c r="B241" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="242" spans="2:2">
+    <row r="242" spans="1:2">
+      <c r="A242" t="s">
+        <v>887</v>
+      </c>
       <c r="B242" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="243" spans="2:2">
+    <row r="243" spans="1:2">
+      <c r="A243" t="s">
+        <v>885</v>
+      </c>
       <c r="B243" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="244" spans="2:2">
+    <row r="244" spans="1:2">
+      <c r="A244" t="s">
+        <v>885</v>
+      </c>
       <c r="B244" t="s">
         <v>744</v>
       </c>
     </row>
-    <row r="245" spans="2:2">
+    <row r="245" spans="1:2">
+      <c r="A245" t="s">
+        <v>887</v>
+      </c>
       <c r="B245" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="246" spans="2:2">
+    <row r="246" spans="1:2">
+      <c r="A246" t="s">
+        <v>885</v>
+      </c>
       <c r="B246" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="247" spans="2:2">
+    <row r="247" spans="1:2">
+      <c r="A247" t="s">
+        <v>885</v>
+      </c>
       <c r="B247" t="s">
         <v>856</v>
       </c>
     </row>
-    <row r="248" spans="2:2">
+    <row r="248" spans="1:2">
+      <c r="A248" t="s">
+        <v>887</v>
+      </c>
       <c r="B248" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="249" spans="2:2">
+    <row r="249" spans="1:2">
+      <c r="A249" t="s">
+        <v>885</v>
+      </c>
       <c r="B249" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="250" spans="2:2">
+    <row r="250" spans="1:2">
+      <c r="A250" t="s">
+        <v>887</v>
+      </c>
       <c r="B250" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="251" spans="2:2">
+    <row r="251" spans="1:2">
+      <c r="A251" t="s">
+        <v>885</v>
+      </c>
       <c r="B251" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="252" spans="2:2">
+    <row r="252" spans="1:2">
+      <c r="A252" t="s">
+        <v>885</v>
+      </c>
       <c r="B252" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="253" spans="2:2">
+    <row r="253" spans="1:2">
+      <c r="A253" t="s">
+        <v>885</v>
+      </c>
       <c r="B253" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="254" spans="2:2">
+    <row r="254" spans="1:2">
+      <c r="A254" t="s">
+        <v>885</v>
+      </c>
       <c r="B254" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="255" spans="2:2">
+    <row r="255" spans="1:2">
+      <c r="A255" t="s">
+        <v>885</v>
+      </c>
       <c r="B255" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="256" spans="2:2">
+    <row r="256" spans="1:2">
+      <c r="A256" t="s">
+        <v>885</v>
+      </c>
       <c r="B256" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="257" spans="2:2">
+    <row r="257" spans="1:2">
+      <c r="A257" t="s">
+        <v>885</v>
+      </c>
       <c r="B257" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="258" spans="2:2">
+    <row r="258" spans="1:2">
+      <c r="A258" t="s">
+        <v>885</v>
+      </c>
       <c r="B258" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="259" spans="2:2">
+    <row r="259" spans="1:2">
+      <c r="A259" t="s">
+        <v>885</v>
+      </c>
       <c r="B259" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="260" spans="2:2">
+    <row r="260" spans="1:2">
+      <c r="A260" t="s">
+        <v>885</v>
+      </c>
       <c r="B260" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="261" spans="2:2">
+    <row r="261" spans="1:2">
+      <c r="A261" t="s">
+        <v>885</v>
+      </c>
       <c r="B261" t="s">
         <v>674</v>
       </c>
     </row>
-    <row r="262" spans="2:2">
+    <row r="262" spans="1:2">
+      <c r="A262" t="s">
+        <v>885</v>
+      </c>
       <c r="B262" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="263" spans="2:2">
+    <row r="263" spans="1:2">
+      <c r="A263" t="s">
+        <v>885</v>
+      </c>
       <c r="B263" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="264" spans="2:2">
+    <row r="264" spans="1:2">
+      <c r="A264" t="s">
+        <v>885</v>
+      </c>
       <c r="B264" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="265" spans="2:2">
+    <row r="265" spans="1:2">
+      <c r="A265" t="s">
+        <v>885</v>
+      </c>
       <c r="B265" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="266" spans="2:2">
+    <row r="266" spans="1:2">
+      <c r="A266" t="s">
+        <v>885</v>
+      </c>
       <c r="B266" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="267" spans="2:2">
+    <row r="267" spans="1:2">
+      <c r="A267" t="s">
+        <v>885</v>
+      </c>
       <c r="B267" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="268" spans="2:2">
+    <row r="268" spans="1:2">
+      <c r="A268" t="s">
+        <v>885</v>
+      </c>
       <c r="B268" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="269" spans="2:2">
+    <row r="269" spans="1:2">
+      <c r="A269" t="s">
+        <v>885</v>
+      </c>
       <c r="B269" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="270" spans="2:2">
+    <row r="270" spans="1:2">
+      <c r="A270" t="s">
+        <v>885</v>
+      </c>
       <c r="B270" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="271" spans="2:2">
+    <row r="271" spans="1:2">
+      <c r="A271" t="s">
+        <v>885</v>
+      </c>
       <c r="B271" t="s">
         <v>771</v>
       </c>
     </row>
-    <row r="272" spans="2:2">
+    <row r="272" spans="1:2">
+      <c r="A272" t="s">
+        <v>885</v>
+      </c>
       <c r="B272" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="273" spans="2:2">
+    <row r="273" spans="1:2">
+      <c r="A273" t="s">
+        <v>885</v>
+      </c>
       <c r="B273" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="274" spans="2:2">
+    <row r="274" spans="1:2">
+      <c r="A274" t="s">
+        <v>885</v>
+      </c>
       <c r="B274" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="275" spans="2:2">
+    <row r="275" spans="1:2">
+      <c r="A275" t="s">
+        <v>885</v>
+      </c>
       <c r="B275" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="276" spans="2:2">
+    <row r="276" spans="1:2">
+      <c r="A276" t="s">
+        <v>885</v>
+      </c>
       <c r="B276" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="277" spans="2:2">
+    <row r="277" spans="1:2">
+      <c r="A277" t="s">
+        <v>885</v>
+      </c>
       <c r="B277" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="278" spans="2:2">
+    <row r="278" spans="1:2">
+      <c r="A278" t="s">
+        <v>885</v>
+      </c>
       <c r="B278" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="279" spans="2:2">
+    <row r="279" spans="1:2">
+      <c r="A279" t="s">
+        <v>885</v>
+      </c>
       <c r="B279" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="280" spans="2:2">
+    <row r="280" spans="1:2">
+      <c r="A280" t="s">
+        <v>885</v>
+      </c>
       <c r="B280" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="281" spans="2:2">
+    <row r="281" spans="1:2">
+      <c r="A281" t="s">
+        <v>885</v>
+      </c>
       <c r="B281" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="282" spans="2:2">
+    <row r="282" spans="1:2">
+      <c r="A282" t="s">
+        <v>885</v>
+      </c>
       <c r="B282" t="s">
         <v>768</v>
       </c>
     </row>
-    <row r="283" spans="2:2">
+    <row r="283" spans="1:2">
+      <c r="A283" t="s">
+        <v>885</v>
+      </c>
       <c r="B283" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="284" spans="2:2">
+    <row r="284" spans="1:2">
+      <c r="A284" t="s">
+        <v>887</v>
+      </c>
       <c r="B284" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="285" spans="2:2">
+    <row r="285" spans="1:2">
+      <c r="A285" t="s">
+        <v>887</v>
+      </c>
       <c r="B285" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="286" spans="2:2">
+    <row r="286" spans="1:2">
+      <c r="A286" t="s">
+        <v>887</v>
+      </c>
       <c r="B286" t="s">
         <v>875</v>
       </c>
     </row>
-    <row r="287" spans="2:2">
+    <row r="287" spans="1:2">
+      <c r="A287" t="s">
+        <v>885</v>
+      </c>
       <c r="B287" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="288" spans="2:2">
+    <row r="288" spans="1:2">
+      <c r="A288" t="s">
+        <v>885</v>
+      </c>
       <c r="B288" t="s">
         <v>829</v>
       </c>
     </row>
-    <row r="289" spans="2:2">
+    <row r="289" spans="1:2">
+      <c r="A289" t="s">
+        <v>887</v>
+      </c>
       <c r="B289" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="290" spans="2:2">
+    <row r="290" spans="1:2">
+      <c r="A290" t="s">
+        <v>885</v>
+      </c>
       <c r="B290" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="291" spans="2:2">
+    <row r="291" spans="1:2">
+      <c r="A291" t="s">
+        <v>885</v>
+      </c>
       <c r="B291" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="292" spans="2:2">
+    <row r="292" spans="1:2">
+      <c r="A292" t="s">
+        <v>885</v>
+      </c>
       <c r="B292" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="293" spans="2:2">
+    <row r="293" spans="1:2">
+      <c r="A293" t="s">
+        <v>885</v>
+      </c>
       <c r="B293" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="294" spans="2:2">
+    <row r="294" spans="1:2">
+      <c r="A294" t="s">
+        <v>885</v>
+      </c>
       <c r="B294" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="295" spans="2:2">
+    <row r="295" spans="1:2">
+      <c r="A295" t="s">
+        <v>885</v>
+      </c>
       <c r="B295" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="296" spans="2:2">
+    <row r="296" spans="1:2">
+      <c r="A296" t="s">
+        <v>885</v>
+      </c>
       <c r="B296" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="297" spans="2:2">
+    <row r="297" spans="1:2">
+      <c r="A297" t="s">
+        <v>885</v>
+      </c>
       <c r="B297" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="298" spans="2:2">
+    <row r="298" spans="1:2">
+      <c r="A298" t="s">
+        <v>885</v>
+      </c>
       <c r="B298" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="299" spans="2:2">
+    <row r="299" spans="1:2">
+      <c r="A299" t="s">
+        <v>885</v>
+      </c>
       <c r="B299" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="300" spans="2:2">
+    <row r="300" spans="1:2">
+      <c r="A300" t="s">
+        <v>885</v>
+      </c>
       <c r="B300" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="301" spans="2:2">
+    <row r="301" spans="1:2">
+      <c r="A301" t="s">
+        <v>885</v>
+      </c>
       <c r="B301" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="302" spans="2:2">
+    <row r="302" spans="1:2">
+      <c r="A302" t="s">
+        <v>885</v>
+      </c>
       <c r="B302" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="303" spans="2:2">
+    <row r="303" spans="1:2">
+      <c r="A303" t="s">
+        <v>885</v>
+      </c>
       <c r="B303" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="304" spans="2:2">
+    <row r="304" spans="1:2">
+      <c r="A304" t="s">
+        <v>885</v>
+      </c>
       <c r="B304" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="305" spans="2:2">
+    <row r="305" spans="1:2">
+      <c r="A305" t="s">
+        <v>887</v>
+      </c>
       <c r="B305" t="s">
         <v>835</v>
       </c>
     </row>
-    <row r="306" spans="2:2">
+    <row r="306" spans="1:2">
+      <c r="A306" t="s">
+        <v>887</v>
+      </c>
       <c r="B306" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="307" spans="2:2">
+    <row r="307" spans="1:2">
+      <c r="A307" t="s">
+        <v>885</v>
+      </c>
       <c r="B307" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="308" spans="2:2">
+    <row r="308" spans="1:2">
+      <c r="A308" t="s">
+        <v>885</v>
+      </c>
       <c r="B308" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="309" spans="2:2">
+    <row r="309" spans="1:2">
+      <c r="A309" t="s">
+        <v>887</v>
+      </c>
       <c r="B309" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="310" spans="2:2">
+    <row r="310" spans="1:2">
+      <c r="A310" t="s">
+        <v>885</v>
+      </c>
       <c r="B310" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="311" spans="2:2">
+    <row r="311" spans="1:2">
+      <c r="A311" t="s">
+        <v>885</v>
+      </c>
       <c r="B311" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="312" spans="2:2">
+    <row r="312" spans="1:2">
+      <c r="A312" t="s">
+        <v>885</v>
+      </c>
       <c r="B312" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="313" spans="2:2">
+    <row r="313" spans="1:2">
+      <c r="A313" t="s">
+        <v>885</v>
+      </c>
       <c r="B313" t="s">
         <v>787</v>
       </c>
     </row>
-    <row r="314" spans="2:2">
+    <row r="314" spans="1:2">
+      <c r="A314" t="s">
+        <v>887</v>
+      </c>
       <c r="B314" t="s">
         <v>788</v>
       </c>
     </row>
-    <row r="315" spans="2:2">
+    <row r="315" spans="1:2">
+      <c r="A315" t="s">
+        <v>885</v>
+      </c>
       <c r="B315" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="316" spans="2:2">
+    <row r="316" spans="1:2">
+      <c r="A316" t="s">
+        <v>885</v>
+      </c>
       <c r="B316" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="317" spans="2:2">
+    <row r="317" spans="1:2">
+      <c r="A317" t="s">
+        <v>885</v>
+      </c>
       <c r="B317" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="318" spans="2:2">
+    <row r="318" spans="1:2">
+      <c r="A318" t="s">
+        <v>885</v>
+      </c>
       <c r="B318" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="319" spans="2:2">
+    <row r="319" spans="1:2">
+      <c r="A319" t="s">
+        <v>885</v>
+      </c>
       <c r="B319" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="320" spans="2:2">
+    <row r="320" spans="1:2">
+      <c r="A320" t="s">
+        <v>885</v>
+      </c>
       <c r="B320" t="s">
         <v>857</v>
       </c>
     </row>
-    <row r="321" spans="2:2">
+    <row r="321" spans="1:2">
+      <c r="A321" t="s">
+        <v>885</v>
+      </c>
       <c r="B321" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="322" spans="2:2">
+    <row r="322" spans="1:2">
+      <c r="A322" t="s">
+        <v>885</v>
+      </c>
       <c r="B322" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="323" spans="2:2">
+    <row r="323" spans="1:2">
+      <c r="A323" t="s">
+        <v>885</v>
+      </c>
       <c r="B323" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="324" spans="2:2">
+    <row r="324" spans="1:2">
+      <c r="A324" t="s">
+        <v>885</v>
+      </c>
       <c r="B324" t="s">
         <v>789</v>
       </c>
     </row>
-    <row r="325" spans="2:2">
+    <row r="325" spans="1:2">
+      <c r="A325" t="s">
+        <v>885</v>
+      </c>
       <c r="B325" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="326" spans="2:2">
+    <row r="326" spans="1:2">
+      <c r="A326" t="s">
+        <v>885</v>
+      </c>
       <c r="B326" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="327" spans="2:2">
+    <row r="327" spans="1:2">
+      <c r="A327" t="s">
+        <v>887</v>
+      </c>
       <c r="B327" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="328" spans="2:2">
+    <row r="328" spans="1:2">
+      <c r="A328" t="s">
+        <v>885</v>
+      </c>
       <c r="B328" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="329" spans="2:2">
+    <row r="329" spans="1:2">
+      <c r="A329" t="s">
+        <v>885</v>
+      </c>
       <c r="B329" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="330" spans="2:2">
+    <row r="330" spans="1:2">
+      <c r="A330" t="s">
+        <v>885</v>
+      </c>
       <c r="B330" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="331" spans="2:2">
+    <row r="331" spans="1:2">
+      <c r="A331" t="s">
+        <v>885</v>
+      </c>
       <c r="B331" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="332" spans="2:2">
+    <row r="332" spans="1:2">
+      <c r="A332" t="s">
+        <v>885</v>
+      </c>
       <c r="B332" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="333" spans="2:2">
+    <row r="333" spans="1:2">
+      <c r="A333" t="s">
+        <v>885</v>
+      </c>
       <c r="B333" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="334" spans="2:2">
+    <row r="334" spans="1:2">
+      <c r="A334" t="s">
+        <v>885</v>
+      </c>
       <c r="B334" t="s">
         <v>761</v>
       </c>
     </row>
-    <row r="335" spans="2:2">
+    <row r="335" spans="1:2">
       <c r="B335" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="336" spans="2:2">
+    <row r="336" spans="1:2">
       <c r="B336" t="s">
         <v>289</v>
       </c>

</xml_diff>

<commit_message>
finally finished mendeley abstracts!
</commit_message>
<xml_diff>
--- a/abstracts.xlsx
+++ b/abstracts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac924\Documents\GitHub\LAB2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A988AAE0-184F-4470-B0FF-F87A2E61CFA0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0CC8CD-A5ED-4EF7-B0BF-10D6FB328B06}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{52E4A73F-0506-324F-90E4-F45C75E5528B}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="888">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="888">
   <si>
     <t>Zettersten, A., &amp; Kučera, H. (1978). A word-frequency list based on American English press reportage. Retrieved from https://scholar.google.com/scholar?hl=en&amp;as_sdt=0%2C25&amp;q=A+word-frequency+list+based+on+American+English+press+reportage&amp;btnG=</t>
   </si>
@@ -31607,8 +31607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0998DB5B-4846-834A-B712-19266A922CC0}">
   <dimension ref="A1:B886"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A521" workbookViewId="0">
-      <selection activeCell="A534" sqref="A534"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
@@ -33070,17 +33070,11 @@
       </c>
     </row>
     <row r="183" spans="1:2">
-      <c r="A183" t="s">
-        <v>885</v>
-      </c>
       <c r="B183" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="184" spans="1:2">
-      <c r="A184" t="s">
-        <v>885</v>
-      </c>
       <c r="B184" t="s">
         <v>115</v>
       </c>
@@ -33686,9 +33680,6 @@
       </c>
     </row>
     <row r="260" spans="1:2">
-      <c r="A260" t="s">
-        <v>885</v>
-      </c>
       <c r="B260" t="s">
         <v>143</v>
       </c>
@@ -34942,9 +34933,6 @@
       </c>
     </row>
     <row r="417" spans="1:2">
-      <c r="A417" t="s">
-        <v>885</v>
-      </c>
       <c r="B417" t="s">
         <v>140</v>
       </c>
@@ -35238,9 +35226,6 @@
       </c>
     </row>
     <row r="454" spans="1:2">
-      <c r="A454" t="s">
-        <v>885</v>
-      </c>
       <c r="B454" t="s">
         <v>139</v>
       </c>
@@ -35326,9 +35311,6 @@
       </c>
     </row>
     <row r="465" spans="1:2">
-      <c r="A465" t="s">
-        <v>885</v>
-      </c>
       <c r="B465" t="s">
         <v>138</v>
       </c>
@@ -35518,9 +35500,6 @@
       </c>
     </row>
     <row r="489" spans="1:2">
-      <c r="A489" t="s">
-        <v>885</v>
-      </c>
       <c r="B489" t="s">
         <v>137</v>
       </c>
@@ -35878,1766 +35857,2771 @@
       </c>
     </row>
     <row r="534" spans="1:2">
+      <c r="A534" t="s">
+        <v>887</v>
+      </c>
       <c r="B534" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="535" spans="1:2">
+      <c r="A535" t="s">
+        <v>885</v>
+      </c>
       <c r="B535" t="s">
         <v>722</v>
       </c>
     </row>
     <row r="536" spans="1:2">
+      <c r="A536" t="s">
+        <v>885</v>
+      </c>
       <c r="B536" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="537" spans="1:2">
+      <c r="A537" t="s">
+        <v>885</v>
+      </c>
       <c r="B537" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="538" spans="1:2">
+      <c r="A538" t="s">
+        <v>885</v>
+      </c>
       <c r="B538" t="s">
         <v>838</v>
       </c>
     </row>
     <row r="539" spans="1:2">
+      <c r="A539" t="s">
+        <v>887</v>
+      </c>
       <c r="B539" t="s">
         <v>840</v>
       </c>
     </row>
     <row r="540" spans="1:2">
+      <c r="A540" t="s">
+        <v>887</v>
+      </c>
       <c r="B540" t="s">
         <v>839</v>
       </c>
     </row>
     <row r="541" spans="1:2">
+      <c r="A541" t="s">
+        <v>887</v>
+      </c>
       <c r="B541" t="s">
         <v>846</v>
       </c>
     </row>
     <row r="542" spans="1:2">
+      <c r="A542" t="s">
+        <v>885</v>
+      </c>
       <c r="B542" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="543" spans="1:2">
+      <c r="A543" t="s">
+        <v>885</v>
+      </c>
       <c r="B543" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="544" spans="1:2">
+      <c r="A544" t="s">
+        <v>885</v>
+      </c>
       <c r="B544" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="545" spans="2:2">
+    <row r="545" spans="1:2">
+      <c r="A545" t="s">
+        <v>885</v>
+      </c>
       <c r="B545" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="546" spans="2:2">
+    <row r="546" spans="1:2">
+      <c r="A546" t="s">
+        <v>885</v>
+      </c>
       <c r="B546" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="547" spans="2:2">
+    <row r="547" spans="1:2">
+      <c r="A547" t="s">
+        <v>885</v>
+      </c>
       <c r="B547" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="548" spans="2:2">
+    <row r="548" spans="1:2">
+      <c r="A548" t="s">
+        <v>885</v>
+      </c>
       <c r="B548" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="549" spans="2:2">
+    <row r="549" spans="1:2">
+      <c r="A549" t="s">
+        <v>885</v>
+      </c>
       <c r="B549" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="550" spans="2:2">
+    <row r="550" spans="1:2">
+      <c r="A550" t="s">
+        <v>887</v>
+      </c>
       <c r="B550" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="551" spans="2:2">
+    <row r="551" spans="1:2">
+      <c r="A551" t="s">
+        <v>885</v>
+      </c>
       <c r="B551" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="552" spans="2:2">
+    <row r="552" spans="1:2">
+      <c r="A552" t="s">
+        <v>887</v>
+      </c>
       <c r="B552" t="s">
         <v>877</v>
       </c>
     </row>
-    <row r="553" spans="2:2">
+    <row r="553" spans="1:2">
+      <c r="A553" t="s">
+        <v>885</v>
+      </c>
       <c r="B553" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="554" spans="2:2">
+    <row r="554" spans="1:2">
+      <c r="A554" t="s">
+        <v>885</v>
+      </c>
       <c r="B554" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="555" spans="2:2">
+    <row r="555" spans="1:2">
+      <c r="A555" t="s">
+        <v>885</v>
+      </c>
       <c r="B555" t="s">
         <v>866</v>
       </c>
     </row>
-    <row r="556" spans="2:2">
+    <row r="556" spans="1:2">
+      <c r="A556" t="s">
+        <v>885</v>
+      </c>
       <c r="B556" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="557" spans="2:2">
+    <row r="557" spans="1:2">
+      <c r="A557" t="s">
+        <v>885</v>
+      </c>
       <c r="B557" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="558" spans="2:2">
+    <row r="558" spans="1:2">
+      <c r="A558" t="s">
+        <v>885</v>
+      </c>
       <c r="B558" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="559" spans="2:2">
+    <row r="559" spans="1:2">
+      <c r="A559" t="s">
+        <v>885</v>
+      </c>
       <c r="B559" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="560" spans="2:2">
+    <row r="560" spans="1:2">
+      <c r="A560" t="s">
+        <v>885</v>
+      </c>
       <c r="B560" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="561" spans="2:2">
+    <row r="561" spans="1:2">
+      <c r="A561" t="s">
+        <v>885</v>
+      </c>
       <c r="B561" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="562" spans="2:2">
+    <row r="562" spans="1:2">
+      <c r="A562" t="s">
+        <v>885</v>
+      </c>
       <c r="B562" t="s">
         <v>863</v>
       </c>
     </row>
-    <row r="563" spans="2:2">
+    <row r="563" spans="1:2">
+      <c r="A563" t="s">
+        <v>885</v>
+      </c>
       <c r="B563" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="564" spans="2:2">
+    <row r="564" spans="1:2">
+      <c r="A564" t="s">
+        <v>885</v>
+      </c>
       <c r="B564" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="565" spans="2:2">
+    <row r="565" spans="1:2">
+      <c r="A565" t="s">
+        <v>885</v>
+      </c>
       <c r="B565" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="566" spans="2:2">
+    <row r="566" spans="1:2">
+      <c r="A566" t="s">
+        <v>887</v>
+      </c>
       <c r="B566" t="s">
         <v>872</v>
       </c>
     </row>
-    <row r="567" spans="2:2">
+    <row r="567" spans="1:2">
+      <c r="A567" t="s">
+        <v>885</v>
+      </c>
       <c r="B567" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="568" spans="2:2">
+    <row r="568" spans="1:2">
+      <c r="A568" t="s">
+        <v>885</v>
+      </c>
       <c r="B568" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="569" spans="2:2">
+    <row r="569" spans="1:2">
+      <c r="A569" t="s">
+        <v>885</v>
+      </c>
       <c r="B569" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="570" spans="2:2">
+    <row r="570" spans="1:2">
+      <c r="A570" t="s">
+        <v>885</v>
+      </c>
       <c r="B570" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="571" spans="2:2">
+    <row r="571" spans="1:2">
+      <c r="A571" t="s">
+        <v>885</v>
+      </c>
       <c r="B571" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="572" spans="2:2">
+    <row r="572" spans="1:2">
+      <c r="A572" t="s">
+        <v>885</v>
+      </c>
       <c r="B572" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="573" spans="2:2">
+    <row r="573" spans="1:2">
+      <c r="A573" t="s">
+        <v>887</v>
+      </c>
       <c r="B573" t="s">
         <v>752</v>
       </c>
     </row>
-    <row r="574" spans="2:2">
+    <row r="574" spans="1:2">
+      <c r="A574" t="s">
+        <v>885</v>
+      </c>
       <c r="B574" t="s">
         <v>810</v>
       </c>
     </row>
-    <row r="575" spans="2:2">
+    <row r="575" spans="1:2">
+      <c r="A575" t="s">
+        <v>885</v>
+      </c>
       <c r="B575" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="576" spans="2:2">
+    <row r="576" spans="1:2">
+      <c r="A576" t="s">
+        <v>887</v>
+      </c>
       <c r="B576" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="577" spans="2:2">
+    <row r="577" spans="1:2">
+      <c r="A577" t="s">
+        <v>885</v>
+      </c>
       <c r="B577" t="s">
         <v>861</v>
       </c>
     </row>
-    <row r="578" spans="2:2">
+    <row r="578" spans="1:2">
+      <c r="A578" t="s">
+        <v>885</v>
+      </c>
       <c r="B578" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="579" spans="2:2">
+    <row r="579" spans="1:2">
+      <c r="A579" t="s">
+        <v>885</v>
+      </c>
       <c r="B579" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="580" spans="2:2">
+    <row r="580" spans="1:2">
+      <c r="A580" t="s">
+        <v>885</v>
+      </c>
       <c r="B580" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="581" spans="2:2">
+    <row r="581" spans="1:2">
+      <c r="A581" t="s">
+        <v>885</v>
+      </c>
       <c r="B581" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="582" spans="2:2">
+    <row r="582" spans="1:2">
+      <c r="A582" t="s">
+        <v>885</v>
+      </c>
       <c r="B582" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="583" spans="2:2">
+    <row r="583" spans="1:2">
+      <c r="A583" t="s">
+        <v>885</v>
+      </c>
       <c r="B583" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="584" spans="2:2">
+    <row r="584" spans="1:2">
+      <c r="A584" t="s">
+        <v>885</v>
+      </c>
       <c r="B584" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="585" spans="2:2">
+    <row r="585" spans="1:2">
+      <c r="A585" t="s">
+        <v>887</v>
+      </c>
       <c r="B585" t="s">
         <v>757</v>
       </c>
     </row>
-    <row r="586" spans="2:2">
+    <row r="586" spans="1:2">
+      <c r="A586" t="s">
+        <v>885</v>
+      </c>
       <c r="B586" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="587" spans="2:2">
+    <row r="587" spans="1:2">
+      <c r="A587" t="s">
+        <v>885</v>
+      </c>
       <c r="B587" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="588" spans="2:2">
+    <row r="588" spans="1:2">
       <c r="B588" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="589" spans="2:2">
+    <row r="589" spans="1:2">
+      <c r="A589" t="s">
+        <v>885</v>
+      </c>
       <c r="B589" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="590" spans="2:2">
+    <row r="590" spans="1:2">
+      <c r="A590" t="s">
+        <v>885</v>
+      </c>
       <c r="B590" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="591" spans="2:2">
+    <row r="591" spans="1:2">
+      <c r="A591" t="s">
+        <v>885</v>
+      </c>
       <c r="B591" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="592" spans="2:2">
+    <row r="592" spans="1:2">
+      <c r="A592" t="s">
+        <v>885</v>
+      </c>
       <c r="B592" t="s">
         <v>737</v>
       </c>
     </row>
-    <row r="593" spans="2:2">
+    <row r="593" spans="1:2">
+      <c r="A593" t="s">
+        <v>887</v>
+      </c>
       <c r="B593" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="594" spans="2:2">
+    <row r="594" spans="1:2">
       <c r="B594" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="595" spans="2:2">
+    <row r="595" spans="1:2">
+      <c r="A595" t="s">
+        <v>885</v>
+      </c>
       <c r="B595" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="596" spans="2:2">
+    <row r="596" spans="1:2">
+      <c r="A596" t="s">
+        <v>885</v>
+      </c>
       <c r="B596" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="597" spans="2:2">
+    <row r="597" spans="1:2">
+      <c r="A597" t="s">
+        <v>885</v>
+      </c>
       <c r="B597" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="598" spans="2:2" ht="18">
+    <row r="598" spans="1:2" ht="18">
+      <c r="A598" t="s">
+        <v>885</v>
+      </c>
       <c r="B598" t="s">
         <v>745</v>
       </c>
     </row>
-    <row r="599" spans="2:2">
+    <row r="599" spans="1:2">
+      <c r="A599" t="s">
+        <v>885</v>
+      </c>
       <c r="B599" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="600" spans="2:2">
+    <row r="600" spans="1:2">
+      <c r="A600" t="s">
+        <v>885</v>
+      </c>
       <c r="B600" t="s">
         <v>675</v>
       </c>
     </row>
-    <row r="601" spans="2:2">
+    <row r="601" spans="1:2">
+      <c r="A601" t="s">
+        <v>887</v>
+      </c>
       <c r="B601" t="s">
         <v>883</v>
       </c>
     </row>
-    <row r="602" spans="2:2">
+    <row r="602" spans="1:2">
+      <c r="A602" t="s">
+        <v>885</v>
+      </c>
       <c r="B602" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="603" spans="2:2">
+    <row r="603" spans="1:2">
+      <c r="A603" t="s">
+        <v>885</v>
+      </c>
       <c r="B603" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="604" spans="2:2">
+    <row r="604" spans="1:2">
+      <c r="A604" t="s">
+        <v>885</v>
+      </c>
       <c r="B604" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="605" spans="2:2">
+    <row r="605" spans="1:2">
+      <c r="A605" t="s">
+        <v>887</v>
+      </c>
       <c r="B605" t="s">
         <v>826</v>
       </c>
     </row>
-    <row r="606" spans="2:2">
+    <row r="606" spans="1:2">
+      <c r="A606" t="s">
+        <v>885</v>
+      </c>
       <c r="B606" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="607" spans="2:2">
+    <row r="607" spans="1:2">
+      <c r="A607" t="s">
+        <v>885</v>
+      </c>
       <c r="B607" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="608" spans="2:2">
+    <row r="608" spans="1:2">
+      <c r="A608" t="s">
+        <v>885</v>
+      </c>
       <c r="B608" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="609" spans="2:2">
+    <row r="609" spans="1:2">
+      <c r="A609" t="s">
+        <v>885</v>
+      </c>
       <c r="B609" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="610" spans="2:2">
+    <row r="610" spans="1:2">
+      <c r="A610" t="s">
+        <v>885</v>
+      </c>
       <c r="B610" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="611" spans="2:2">
+    <row r="611" spans="1:2">
+      <c r="A611" t="s">
+        <v>885</v>
+      </c>
       <c r="B611" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="612" spans="2:2">
+    <row r="612" spans="1:2">
+      <c r="A612" t="s">
+        <v>885</v>
+      </c>
       <c r="B612" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="613" spans="2:2">
+    <row r="613" spans="1:2">
+      <c r="A613" t="s">
+        <v>885</v>
+      </c>
       <c r="B613" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="614" spans="2:2">
+    <row r="614" spans="1:2">
+      <c r="A614" t="s">
+        <v>885</v>
+      </c>
       <c r="B614" t="s">
         <v>841</v>
       </c>
     </row>
-    <row r="615" spans="2:2">
+    <row r="615" spans="1:2">
+      <c r="A615" t="s">
+        <v>885</v>
+      </c>
       <c r="B615" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="616" spans="2:2">
+    <row r="616" spans="1:2">
       <c r="B616" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="617" spans="2:2">
+    <row r="617" spans="1:2">
       <c r="B617" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="618" spans="2:2">
+    <row r="618" spans="1:2">
+      <c r="A618" t="s">
+        <v>885</v>
+      </c>
       <c r="B618" t="s">
         <v>742</v>
       </c>
     </row>
-    <row r="619" spans="2:2">
+    <row r="619" spans="1:2">
+      <c r="A619" t="s">
+        <v>885</v>
+      </c>
       <c r="B619" t="s">
         <v>712</v>
       </c>
     </row>
-    <row r="620" spans="2:2">
+    <row r="620" spans="1:2">
+      <c r="A620" t="s">
+        <v>885</v>
+      </c>
       <c r="B620" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="621" spans="2:2">
+    <row r="621" spans="1:2">
+      <c r="A621" t="s">
+        <v>885</v>
+      </c>
       <c r="B621" t="s">
         <v>723</v>
       </c>
     </row>
-    <row r="622" spans="2:2">
+    <row r="622" spans="1:2">
+      <c r="A622" t="s">
+        <v>885</v>
+      </c>
       <c r="B622" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="623" spans="2:2">
+    <row r="623" spans="1:2">
+      <c r="A623" t="s">
+        <v>885</v>
+      </c>
       <c r="B623" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="624" spans="2:2">
+    <row r="624" spans="1:2">
       <c r="B624" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="625" spans="2:2">
+    <row r="625" spans="1:2">
+      <c r="A625" t="s">
+        <v>885</v>
+      </c>
       <c r="B625" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="626" spans="2:2">
+    <row r="626" spans="1:2">
+      <c r="A626" t="s">
+        <v>885</v>
+      </c>
       <c r="B626" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="627" spans="2:2">
+    <row r="627" spans="1:2">
+      <c r="A627" t="s">
+        <v>887</v>
+      </c>
       <c r="B627" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="628" spans="2:2">
+    <row r="628" spans="1:2">
+      <c r="A628" t="s">
+        <v>885</v>
+      </c>
       <c r="B628" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="629" spans="2:2">
+    <row r="629" spans="1:2">
+      <c r="A629" t="s">
+        <v>885</v>
+      </c>
       <c r="B629" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="630" spans="2:2">
+    <row r="630" spans="1:2">
+      <c r="A630" t="s">
+        <v>885</v>
+      </c>
       <c r="B630" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="631" spans="2:2">
+    <row r="631" spans="1:2">
+      <c r="A631" t="s">
+        <v>885</v>
+      </c>
       <c r="B631" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="632" spans="2:2">
+    <row r="632" spans="1:2">
+      <c r="A632" t="s">
+        <v>885</v>
+      </c>
       <c r="B632" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="633" spans="2:2">
+    <row r="633" spans="1:2">
+      <c r="A633" t="s">
+        <v>885</v>
+      </c>
       <c r="B633" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="634" spans="2:2">
+    <row r="634" spans="1:2">
+      <c r="A634" t="s">
+        <v>885</v>
+      </c>
       <c r="B634" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="635" spans="2:2">
+    <row r="635" spans="1:2">
+      <c r="A635" t="s">
+        <v>887</v>
+      </c>
       <c r="B635" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="636" spans="2:2">
+    <row r="636" spans="1:2">
+      <c r="A636" t="s">
+        <v>885</v>
+      </c>
       <c r="B636" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="637" spans="2:2">
+    <row r="637" spans="1:2">
+      <c r="A637" t="s">
+        <v>885</v>
+      </c>
       <c r="B637" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="638" spans="2:2">
+    <row r="638" spans="1:2">
+      <c r="A638" t="s">
+        <v>885</v>
+      </c>
       <c r="B638" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="639" spans="2:2">
+    <row r="639" spans="1:2">
+      <c r="A639" t="s">
+        <v>885</v>
+      </c>
       <c r="B639" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="640" spans="2:2">
+    <row r="640" spans="1:2">
+      <c r="A640" t="s">
+        <v>885</v>
+      </c>
       <c r="B640" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="641" spans="2:2">
+    <row r="641" spans="1:2">
+      <c r="A641" t="s">
+        <v>885</v>
+      </c>
       <c r="B641" t="s">
         <v>865</v>
       </c>
     </row>
-    <row r="642" spans="2:2">
+    <row r="642" spans="1:2">
+      <c r="A642" t="s">
+        <v>885</v>
+      </c>
       <c r="B642" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="643" spans="2:2">
+    <row r="643" spans="1:2">
+      <c r="A643" t="s">
+        <v>885</v>
+      </c>
       <c r="B643" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="644" spans="2:2">
+    <row r="644" spans="1:2">
+      <c r="A644" t="s">
+        <v>885</v>
+      </c>
       <c r="B644" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="645" spans="2:2">
+    <row r="645" spans="1:2">
+      <c r="A645" t="s">
+        <v>887</v>
+      </c>
       <c r="B645" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="646" spans="2:2">
+    <row r="646" spans="1:2">
+      <c r="A646" t="s">
+        <v>885</v>
+      </c>
       <c r="B646" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="647" spans="2:2">
+    <row r="647" spans="1:2">
+      <c r="A647" t="s">
+        <v>885</v>
+      </c>
       <c r="B647" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="648" spans="2:2">
+    <row r="648" spans="1:2">
+      <c r="A648" t="s">
+        <v>885</v>
+      </c>
       <c r="B648" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="649" spans="2:2">
+    <row r="649" spans="1:2">
+      <c r="A649" t="s">
+        <v>885</v>
+      </c>
       <c r="B649" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="650" spans="2:2">
+    <row r="650" spans="1:2">
+      <c r="A650" t="s">
+        <v>885</v>
+      </c>
       <c r="B650" t="s">
         <v>781</v>
       </c>
     </row>
-    <row r="651" spans="2:2">
+    <row r="651" spans="1:2">
+      <c r="A651" t="s">
+        <v>885</v>
+      </c>
       <c r="B651" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="652" spans="2:2">
+    <row r="652" spans="1:2">
+      <c r="A652" t="s">
+        <v>885</v>
+      </c>
       <c r="B652" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="653" spans="2:2">
+    <row r="653" spans="1:2">
+      <c r="A653" t="s">
+        <v>885</v>
+      </c>
       <c r="B653" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="654" spans="2:2">
+    <row r="654" spans="1:2">
+      <c r="A654" t="s">
+        <v>885</v>
+      </c>
       <c r="B654" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="655" spans="2:2">
+    <row r="655" spans="1:2">
       <c r="B655" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="656" spans="2:2">
+    <row r="656" spans="1:2">
+      <c r="A656" t="s">
+        <v>885</v>
+      </c>
       <c r="B656" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="657" spans="2:2">
+    <row r="657" spans="1:2">
+      <c r="A657" t="s">
+        <v>885</v>
+      </c>
       <c r="B657" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="658" spans="2:2">
+    <row r="658" spans="1:2">
+      <c r="A658" t="s">
+        <v>885</v>
+      </c>
       <c r="B658" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="659" spans="2:2">
+    <row r="659" spans="1:2">
+      <c r="A659" t="s">
+        <v>887</v>
+      </c>
       <c r="B659" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="660" spans="2:2">
+    <row r="660" spans="1:2">
+      <c r="A660" t="s">
+        <v>885</v>
+      </c>
       <c r="B660" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="661" spans="2:2">
+    <row r="661" spans="1:2">
+      <c r="A661" t="s">
+        <v>885</v>
+      </c>
       <c r="B661" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="662" spans="2:2">
+    <row r="662" spans="1:2">
+      <c r="A662" t="s">
+        <v>885</v>
+      </c>
       <c r="B662" t="s">
         <v>859</v>
       </c>
     </row>
-    <row r="663" spans="2:2">
+    <row r="663" spans="1:2">
+      <c r="A663" t="s">
+        <v>885</v>
+      </c>
       <c r="B663" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="664" spans="2:2">
+    <row r="664" spans="1:2">
+      <c r="A664" t="s">
+        <v>885</v>
+      </c>
       <c r="B664" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="665" spans="2:2">
+    <row r="665" spans="1:2">
+      <c r="A665" t="s">
+        <v>885</v>
+      </c>
       <c r="B665" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="666" spans="2:2">
+    <row r="666" spans="1:2">
       <c r="B666" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="667" spans="2:2">
+    <row r="667" spans="1:2">
+      <c r="A667" t="s">
+        <v>885</v>
+      </c>
       <c r="B667" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="668" spans="2:2">
+    <row r="668" spans="1:2">
+      <c r="A668" t="s">
+        <v>885</v>
+      </c>
       <c r="B668" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="669" spans="2:2">
+    <row r="669" spans="1:2">
+      <c r="A669" t="s">
+        <v>885</v>
+      </c>
       <c r="B669" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="670" spans="2:2">
+    <row r="670" spans="1:2">
+      <c r="A670" t="s">
+        <v>885</v>
+      </c>
       <c r="B670" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="671" spans="2:2">
+    <row r="671" spans="1:2">
+      <c r="A671" t="s">
+        <v>885</v>
+      </c>
       <c r="B671" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="672" spans="2:2">
+    <row r="672" spans="1:2">
+      <c r="A672" t="s">
+        <v>885</v>
+      </c>
       <c r="B672" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="673" spans="2:2">
+    <row r="673" spans="1:2">
+      <c r="A673" t="s">
+        <v>887</v>
+      </c>
       <c r="B673" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="674" spans="2:2">
+    <row r="674" spans="1:2">
+      <c r="A674" t="s">
+        <v>885</v>
+      </c>
       <c r="B674" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="675" spans="2:2">
+    <row r="675" spans="1:2">
+      <c r="A675" t="s">
+        <v>885</v>
+      </c>
       <c r="B675" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="676" spans="2:2">
+    <row r="676" spans="1:2">
+      <c r="A676" t="s">
+        <v>885</v>
+      </c>
       <c r="B676" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="677" spans="2:2">
+    <row r="677" spans="1:2">
+      <c r="A677" t="s">
+        <v>885</v>
+      </c>
       <c r="B677" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="678" spans="2:2">
+    <row r="678" spans="1:2">
+      <c r="A678" t="s">
+        <v>885</v>
+      </c>
       <c r="B678" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="679" spans="2:2">
+    <row r="679" spans="1:2">
+      <c r="A679" t="s">
+        <v>885</v>
+      </c>
       <c r="B679" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="680" spans="2:2">
+    <row r="680" spans="1:2">
+      <c r="A680" t="s">
+        <v>885</v>
+      </c>
       <c r="B680" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="681" spans="2:2">
+    <row r="681" spans="1:2">
+      <c r="A681" t="s">
+        <v>885</v>
+      </c>
       <c r="B681" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="682" spans="2:2">
+    <row r="682" spans="1:2">
+      <c r="A682" t="s">
+        <v>885</v>
+      </c>
       <c r="B682" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="683" spans="2:2">
+    <row r="683" spans="1:2">
+      <c r="A683" t="s">
+        <v>885</v>
+      </c>
       <c r="B683" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="684" spans="2:2">
+    <row r="684" spans="1:2">
+      <c r="A684" t="s">
+        <v>885</v>
+      </c>
       <c r="B684" t="s">
         <v>782</v>
       </c>
     </row>
-    <row r="685" spans="2:2">
+    <row r="685" spans="1:2">
+      <c r="A685" t="s">
+        <v>885</v>
+      </c>
       <c r="B685" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="686" spans="2:2">
+    <row r="686" spans="1:2">
+      <c r="A686" t="s">
+        <v>885</v>
+      </c>
       <c r="B686" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="687" spans="2:2">
+    <row r="687" spans="1:2">
+      <c r="A687" t="s">
+        <v>885</v>
+      </c>
       <c r="B687" t="s">
         <v>785</v>
       </c>
     </row>
-    <row r="688" spans="2:2">
+    <row r="688" spans="1:2">
+      <c r="A688" t="s">
+        <v>885</v>
+      </c>
       <c r="B688" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="689" spans="2:2">
+    <row r="689" spans="1:2">
+      <c r="A689" t="s">
+        <v>885</v>
+      </c>
       <c r="B689" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="690" spans="2:2">
+    <row r="690" spans="1:2">
+      <c r="A690" t="s">
+        <v>885</v>
+      </c>
       <c r="B690" t="s">
         <v>783</v>
       </c>
     </row>
-    <row r="691" spans="2:2">
+    <row r="691" spans="1:2">
+      <c r="A691" t="s">
+        <v>885</v>
+      </c>
       <c r="B691" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="692" spans="2:2">
+    <row r="692" spans="1:2">
+      <c r="A692" t="s">
+        <v>885</v>
+      </c>
       <c r="B692" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="693" spans="2:2">
+    <row r="693" spans="1:2">
+      <c r="A693" t="s">
+        <v>885</v>
+      </c>
       <c r="B693" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="694" spans="2:2">
+    <row r="694" spans="1:2">
+      <c r="A694" t="s">
+        <v>885</v>
+      </c>
       <c r="B694" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="695" spans="2:2">
+    <row r="695" spans="1:2">
+      <c r="A695" t="s">
+        <v>887</v>
+      </c>
       <c r="B695" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="696" spans="2:2">
+    <row r="696" spans="1:2">
+      <c r="A696" t="s">
+        <v>885</v>
+      </c>
       <c r="B696" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="697" spans="2:2">
+    <row r="697" spans="1:2">
+      <c r="A697" t="s">
+        <v>885</v>
+      </c>
       <c r="B697" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="698" spans="2:2">
+    <row r="698" spans="1:2">
+      <c r="A698" t="s">
+        <v>885</v>
+      </c>
       <c r="B698" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="699" spans="2:2">
+    <row r="699" spans="1:2">
+      <c r="A699" t="s">
+        <v>885</v>
+      </c>
       <c r="B699" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="700" spans="2:2">
+    <row r="700" spans="1:2">
+      <c r="A700" t="s">
+        <v>885</v>
+      </c>
       <c r="B700" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="701" spans="2:2">
+    <row r="701" spans="1:2">
+      <c r="A701" t="s">
+        <v>885</v>
+      </c>
       <c r="B701" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="702" spans="2:2">
+    <row r="702" spans="1:2">
+      <c r="A702" t="s">
+        <v>885</v>
+      </c>
       <c r="B702" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="703" spans="2:2">
+    <row r="703" spans="1:2">
+      <c r="A703" t="s">
+        <v>885</v>
+      </c>
       <c r="B703" t="s">
         <v>816</v>
       </c>
     </row>
-    <row r="704" spans="2:2">
+    <row r="704" spans="1:2">
+      <c r="A704" t="s">
+        <v>885</v>
+      </c>
       <c r="B704" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="705" spans="2:2">
+    <row r="705" spans="1:2">
+      <c r="A705" t="s">
+        <v>885</v>
+      </c>
       <c r="B705" t="s">
         <v>817</v>
       </c>
     </row>
-    <row r="706" spans="2:2">
+    <row r="706" spans="1:2">
+      <c r="A706" t="s">
+        <v>885</v>
+      </c>
       <c r="B706" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="707" spans="2:2">
+    <row r="707" spans="1:2">
+      <c r="A707" t="s">
+        <v>887</v>
+      </c>
       <c r="B707" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="708" spans="2:2">
+    <row r="708" spans="1:2">
+      <c r="A708" t="s">
+        <v>885</v>
+      </c>
       <c r="B708" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="709" spans="2:2">
+    <row r="709" spans="1:2">
+      <c r="A709" t="s">
+        <v>885</v>
+      </c>
       <c r="B709" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="710" spans="2:2">
+    <row r="710" spans="1:2">
+      <c r="A710" t="s">
+        <v>885</v>
+      </c>
       <c r="B710" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="711" spans="2:2">
+    <row r="711" spans="1:2">
+      <c r="A711" t="s">
+        <v>885</v>
+      </c>
       <c r="B711" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="712" spans="2:2">
+    <row r="712" spans="1:2">
+      <c r="A712" t="s">
+        <v>885</v>
+      </c>
       <c r="B712" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="713" spans="2:2">
+    <row r="713" spans="1:2">
+      <c r="A713" t="s">
+        <v>885</v>
+      </c>
       <c r="B713" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="714" spans="2:2">
+    <row r="714" spans="1:2">
+      <c r="A714" t="s">
+        <v>885</v>
+      </c>
       <c r="B714" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="715" spans="2:2">
+    <row r="715" spans="1:2">
+      <c r="A715" t="s">
+        <v>885</v>
+      </c>
       <c r="B715" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="716" spans="2:2">
+    <row r="716" spans="1:2">
+      <c r="A716" t="s">
+        <v>885</v>
+      </c>
       <c r="B716" t="s">
         <v>849</v>
       </c>
     </row>
-    <row r="717" spans="2:2">
+    <row r="717" spans="1:2">
+      <c r="A717" t="s">
+        <v>887</v>
+      </c>
       <c r="B717" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="718" spans="2:2">
+    <row r="718" spans="1:2">
+      <c r="A718" t="s">
+        <v>887</v>
+      </c>
       <c r="B718" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="719" spans="2:2">
+    <row r="719" spans="1:2">
+      <c r="A719" t="s">
+        <v>885</v>
+      </c>
       <c r="B719" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="720" spans="2:2">
+    <row r="720" spans="1:2">
+      <c r="A720" t="s">
+        <v>885</v>
+      </c>
       <c r="B720" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="721" spans="2:2">
+    <row r="721" spans="1:2">
+      <c r="A721" t="s">
+        <v>885</v>
+      </c>
       <c r="B721" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="722" spans="2:2">
+    <row r="722" spans="1:2">
+      <c r="A722" t="s">
+        <v>885</v>
+      </c>
       <c r="B722" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="723" spans="2:2">
+    <row r="723" spans="1:2">
+      <c r="A723" t="s">
+        <v>885</v>
+      </c>
       <c r="B723" t="s">
         <v>842</v>
       </c>
     </row>
-    <row r="724" spans="2:2">
+    <row r="724" spans="1:2">
+      <c r="A724" t="s">
+        <v>885</v>
+      </c>
       <c r="B724" t="s">
         <v>843</v>
       </c>
     </row>
-    <row r="725" spans="2:2">
+    <row r="725" spans="1:2">
+      <c r="A725" t="s">
+        <v>885</v>
+      </c>
       <c r="B725" t="s">
         <v>850</v>
       </c>
     </row>
-    <row r="726" spans="2:2">
+    <row r="726" spans="1:2">
+      <c r="A726" t="s">
+        <v>885</v>
+      </c>
       <c r="B726" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="727" spans="2:2">
+    <row r="727" spans="1:2">
+      <c r="A727" t="s">
+        <v>885</v>
+      </c>
       <c r="B727" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="728" spans="2:2">
+    <row r="728" spans="1:2">
+      <c r="A728" t="s">
+        <v>885</v>
+      </c>
       <c r="B728" t="s">
         <v>813</v>
       </c>
     </row>
-    <row r="729" spans="2:2">
+    <row r="729" spans="1:2">
+      <c r="A729" t="s">
+        <v>887</v>
+      </c>
       <c r="B729" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="730" spans="2:2">
+    <row r="730" spans="1:2">
+      <c r="A730" t="s">
+        <v>885</v>
+      </c>
       <c r="B730" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="731" spans="2:2">
+    <row r="731" spans="1:2">
+      <c r="A731" t="s">
+        <v>885</v>
+      </c>
       <c r="B731" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="732" spans="2:2">
+    <row r="732" spans="1:2">
+      <c r="A732" t="s">
+        <v>885</v>
+      </c>
       <c r="B732" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="733" spans="2:2">
+    <row r="733" spans="1:2">
       <c r="B733" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="734" spans="2:2">
+    <row r="734" spans="1:2">
+      <c r="A734" t="s">
+        <v>885</v>
+      </c>
       <c r="B734" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="735" spans="2:2">
+    <row r="735" spans="1:2">
+      <c r="A735" t="s">
+        <v>885</v>
+      </c>
       <c r="B735" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="736" spans="2:2">
+    <row r="736" spans="1:2">
+      <c r="A736" t="s">
+        <v>885</v>
+      </c>
       <c r="B736" t="s">
         <v>827</v>
       </c>
     </row>
-    <row r="737" spans="2:2">
+    <row r="737" spans="1:2">
+      <c r="A737" t="s">
+        <v>887</v>
+      </c>
       <c r="B737" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="738" spans="2:2">
+    <row r="738" spans="1:2">
+      <c r="A738" t="s">
+        <v>885</v>
+      </c>
       <c r="B738" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="739" spans="2:2">
+    <row r="739" spans="1:2">
+      <c r="A739" t="s">
+        <v>885</v>
+      </c>
       <c r="B739" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="740" spans="2:2">
+    <row r="740" spans="1:2">
+      <c r="A740" t="s">
+        <v>885</v>
+      </c>
       <c r="B740" t="s">
         <v>718</v>
       </c>
     </row>
-    <row r="741" spans="2:2">
+    <row r="741" spans="1:2">
+      <c r="A741" t="s">
+        <v>885</v>
+      </c>
       <c r="B741" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="742" spans="2:2">
+    <row r="742" spans="1:2">
+      <c r="A742" t="s">
+        <v>885</v>
+      </c>
       <c r="B742" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="743" spans="2:2">
+    <row r="743" spans="1:2">
+      <c r="A743" t="s">
+        <v>885</v>
+      </c>
       <c r="B743" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="744" spans="2:2">
+    <row r="744" spans="1:2">
+      <c r="A744" t="s">
+        <v>885</v>
+      </c>
       <c r="B744" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="745" spans="2:2">
+    <row r="745" spans="1:2">
+      <c r="A745" t="s">
+        <v>885</v>
+      </c>
       <c r="B745" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="746" spans="2:2">
+    <row r="746" spans="1:2">
+      <c r="A746" t="s">
+        <v>885</v>
+      </c>
       <c r="B746" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="747" spans="2:2">
+    <row r="747" spans="1:2">
+      <c r="A747" t="s">
+        <v>885</v>
+      </c>
       <c r="B747" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="748" spans="2:2">
+    <row r="748" spans="1:2">
+      <c r="A748" t="s">
+        <v>885</v>
+      </c>
       <c r="B748" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="749" spans="2:2">
+    <row r="749" spans="1:2">
+      <c r="A749" t="s">
+        <v>885</v>
+      </c>
       <c r="B749" t="s">
         <v>852</v>
       </c>
     </row>
-    <row r="750" spans="2:2">
+    <row r="750" spans="1:2">
+      <c r="A750" t="s">
+        <v>885</v>
+      </c>
       <c r="B750" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="751" spans="2:2">
+    <row r="751" spans="1:2">
+      <c r="A751" t="s">
+        <v>885</v>
+      </c>
       <c r="B751" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="752" spans="2:2">
+    <row r="752" spans="1:2">
+      <c r="A752" t="s">
+        <v>885</v>
+      </c>
       <c r="B752" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="753" spans="2:2">
+    <row r="753" spans="1:2">
+      <c r="A753" t="s">
+        <v>885</v>
+      </c>
       <c r="B753" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="754" spans="2:2">
+    <row r="754" spans="1:2">
+      <c r="A754" t="s">
+        <v>885</v>
+      </c>
       <c r="B754" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="755" spans="2:2">
+    <row r="755" spans="1:2">
+      <c r="A755" t="s">
+        <v>885</v>
+      </c>
       <c r="B755" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="756" spans="2:2">
+    <row r="756" spans="1:2">
+      <c r="A756" t="s">
+        <v>885</v>
+      </c>
       <c r="B756" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="757" spans="2:2">
+    <row r="757" spans="1:2">
+      <c r="A757" t="s">
+        <v>885</v>
+      </c>
       <c r="B757" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="758" spans="2:2">
+    <row r="758" spans="1:2">
+      <c r="A758" t="s">
+        <v>885</v>
+      </c>
       <c r="B758" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="759" spans="2:2">
+    <row r="759" spans="1:2">
+      <c r="A759" t="s">
+        <v>887</v>
+      </c>
       <c r="B759" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="760" spans="2:2">
+    <row r="760" spans="1:2">
+      <c r="A760" t="s">
+        <v>885</v>
+      </c>
       <c r="B760" t="s">
         <v>769</v>
       </c>
     </row>
-    <row r="761" spans="2:2">
+    <row r="761" spans="1:2">
+      <c r="A761" t="s">
+        <v>885</v>
+      </c>
       <c r="B761" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="762" spans="2:2">
+    <row r="762" spans="1:2">
+      <c r="A762" t="s">
+        <v>885</v>
+      </c>
       <c r="B762" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="763" spans="2:2">
+    <row r="763" spans="1:2">
+      <c r="A763" t="s">
+        <v>885</v>
+      </c>
       <c r="B763" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="764" spans="2:2">
+    <row r="764" spans="1:2">
+      <c r="A764" t="s">
+        <v>885</v>
+      </c>
       <c r="B764" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="765" spans="2:2">
+    <row r="765" spans="1:2">
+      <c r="A765" t="s">
+        <v>885</v>
+      </c>
       <c r="B765" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="766" spans="2:2">
+    <row r="766" spans="1:2">
+      <c r="A766" t="s">
+        <v>885</v>
+      </c>
       <c r="B766" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="767" spans="2:2">
+    <row r="767" spans="1:2">
+      <c r="A767" t="s">
+        <v>887</v>
+      </c>
       <c r="B767" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="768" spans="2:2">
+    <row r="768" spans="1:2">
+      <c r="A768" t="s">
+        <v>885</v>
+      </c>
       <c r="B768" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="769" spans="2:2">
+    <row r="769" spans="1:2">
+      <c r="A769" t="s">
+        <v>885</v>
+      </c>
       <c r="B769" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="770" spans="2:2">
+    <row r="770" spans="1:2">
+      <c r="A770" t="s">
+        <v>885</v>
+      </c>
       <c r="B770" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="771" spans="2:2">
+    <row r="771" spans="1:2">
+      <c r="A771" t="s">
+        <v>885</v>
+      </c>
       <c r="B771" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="772" spans="2:2">
+    <row r="772" spans="1:2">
+      <c r="A772" t="s">
+        <v>885</v>
+      </c>
       <c r="B772" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="773" spans="2:2">
+    <row r="773" spans="1:2">
+      <c r="A773" t="s">
+        <v>885</v>
+      </c>
       <c r="B773" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="774" spans="2:2">
+    <row r="774" spans="1:2">
+      <c r="A774" t="s">
+        <v>885</v>
+      </c>
       <c r="B774" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="775" spans="2:2">
+    <row r="775" spans="1:2">
+      <c r="A775" t="s">
+        <v>885</v>
+      </c>
       <c r="B775" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="776" spans="2:2">
+    <row r="776" spans="1:2">
+      <c r="A776" t="s">
+        <v>885</v>
+      </c>
       <c r="B776" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="777" spans="2:2">
+    <row r="777" spans="1:2">
+      <c r="A777" t="s">
+        <v>885</v>
+      </c>
       <c r="B777" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="778" spans="2:2">
+    <row r="778" spans="1:2">
+      <c r="A778" t="s">
+        <v>885</v>
+      </c>
       <c r="B778" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="779" spans="2:2">
+    <row r="779" spans="1:2">
+      <c r="A779" t="s">
+        <v>885</v>
+      </c>
       <c r="B779" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="780" spans="2:2">
+    <row r="780" spans="1:2">
+      <c r="A780" t="s">
+        <v>885</v>
+      </c>
       <c r="B780" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="781" spans="2:2">
+    <row r="781" spans="1:2">
+      <c r="A781" t="s">
+        <v>885</v>
+      </c>
       <c r="B781" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="782" spans="2:2">
+    <row r="782" spans="1:2">
+      <c r="A782" t="s">
+        <v>885</v>
+      </c>
       <c r="B782" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="783" spans="2:2">
+    <row r="783" spans="1:2">
+      <c r="A783" t="s">
+        <v>885</v>
+      </c>
       <c r="B783" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="784" spans="2:2">
+    <row r="784" spans="1:2">
+      <c r="A784" t="s">
+        <v>885</v>
+      </c>
       <c r="B784" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="785" spans="2:2">
+    <row r="785" spans="1:2">
+      <c r="A785" t="s">
+        <v>885</v>
+      </c>
       <c r="B785" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="786" spans="2:2">
+    <row r="786" spans="1:2">
+      <c r="A786" t="s">
+        <v>885</v>
+      </c>
       <c r="B786" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="787" spans="2:2">
+    <row r="787" spans="1:2">
+      <c r="A787" t="s">
+        <v>885</v>
+      </c>
       <c r="B787" t="s">
         <v>828</v>
       </c>
     </row>
-    <row r="788" spans="2:2">
+    <row r="788" spans="1:2">
+      <c r="A788" t="s">
+        <v>885</v>
+      </c>
       <c r="B788" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="789" spans="2:2">
+    <row r="789" spans="1:2">
+      <c r="A789" t="s">
+        <v>885</v>
+      </c>
       <c r="B789" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="790" spans="2:2">
+    <row r="790" spans="1:2">
+      <c r="A790" t="s">
+        <v>885</v>
+      </c>
       <c r="B790" t="s">
         <v>740</v>
       </c>
     </row>
-    <row r="791" spans="2:2">
+    <row r="791" spans="1:2">
+      <c r="A791" t="s">
+        <v>885</v>
+      </c>
       <c r="B791" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="792" spans="2:2">
+    <row r="792" spans="1:2">
+      <c r="A792" t="s">
+        <v>885</v>
+      </c>
       <c r="B792" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="793" spans="2:2">
+    <row r="793" spans="1:2">
       <c r="B793" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="794" spans="2:2">
+    <row r="794" spans="1:2">
       <c r="B794" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="795" spans="2:2">
+    <row r="795" spans="1:2">
+      <c r="A795" t="s">
+        <v>887</v>
+      </c>
       <c r="B795" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="796" spans="2:2">
+    <row r="796" spans="1:2">
       <c r="B796" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="797" spans="2:2">
+    <row r="797" spans="1:2">
+      <c r="A797" t="s">
+        <v>885</v>
+      </c>
       <c r="B797" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="798" spans="2:2">
+    <row r="798" spans="1:2">
+      <c r="A798" t="s">
+        <v>885</v>
+      </c>
       <c r="B798" t="s">
         <v>706</v>
       </c>
     </row>
-    <row r="799" spans="2:2">
+    <row r="799" spans="1:2">
+      <c r="A799" t="s">
+        <v>887</v>
+      </c>
       <c r="B799" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="800" spans="2:2">
+    <row r="800" spans="1:2">
+      <c r="A800" t="s">
+        <v>885</v>
+      </c>
       <c r="B800" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="801" spans="2:2">
+    <row r="801" spans="1:2">
+      <c r="A801" t="s">
+        <v>885</v>
+      </c>
       <c r="B801" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="802" spans="2:2">
+    <row r="802" spans="1:2">
+      <c r="A802" t="s">
+        <v>885</v>
+      </c>
       <c r="B802" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="803" spans="2:2">
+    <row r="803" spans="1:2">
+      <c r="A803" t="s">
+        <v>885</v>
+      </c>
       <c r="B803" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="804" spans="2:2">
+    <row r="804" spans="1:2">
+      <c r="A804" t="s">
+        <v>885</v>
+      </c>
       <c r="B804" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="805" spans="2:2">
+    <row r="805" spans="1:2">
+      <c r="A805" t="s">
+        <v>885</v>
+      </c>
       <c r="B805" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="806" spans="2:2">
+    <row r="806" spans="1:2">
+      <c r="A806" t="s">
+        <v>885</v>
+      </c>
       <c r="B806" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="807" spans="2:2">
+    <row r="807" spans="1:2">
+      <c r="A807" t="s">
+        <v>885</v>
+      </c>
       <c r="B807" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="808" spans="2:2">
+    <row r="808" spans="1:2">
+      <c r="A808" t="s">
+        <v>885</v>
+      </c>
       <c r="B808" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="809" spans="2:2">
+    <row r="809" spans="1:2">
+      <c r="A809" t="s">
+        <v>885</v>
+      </c>
       <c r="B809" t="s">
         <v>853</v>
       </c>
     </row>
-    <row r="810" spans="2:2">
+    <row r="810" spans="1:2">
+      <c r="A810" t="s">
+        <v>885</v>
+      </c>
       <c r="B810" t="s">
         <v>844</v>
       </c>
     </row>
-    <row r="811" spans="2:2">
+    <row r="811" spans="1:2">
+      <c r="A811" t="s">
+        <v>885</v>
+      </c>
       <c r="B811" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="812" spans="2:2">
+    <row r="812" spans="1:2">
+      <c r="A812" t="s">
+        <v>885</v>
+      </c>
       <c r="B812" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="813" spans="2:2">
+    <row r="813" spans="1:2">
+      <c r="A813" t="s">
+        <v>885</v>
+      </c>
       <c r="B813" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="814" spans="2:2">
+    <row r="814" spans="1:2">
+      <c r="A814" t="s">
+        <v>885</v>
+      </c>
       <c r="B814" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="815" spans="2:2">
+    <row r="815" spans="1:2">
+      <c r="A815" t="s">
+        <v>885</v>
+      </c>
       <c r="B815" t="s">
         <v>764</v>
       </c>
     </row>
-    <row r="816" spans="2:2">
+    <row r="816" spans="1:2">
+      <c r="A816" t="s">
+        <v>885</v>
+      </c>
       <c r="B816" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="817" spans="2:2">
+    <row r="817" spans="1:2">
+      <c r="A817" t="s">
+        <v>885</v>
+      </c>
       <c r="B817" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="818" spans="2:2">
+    <row r="818" spans="1:2">
       <c r="B818" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="819" spans="2:2">
+    <row r="819" spans="1:2">
       <c r="B819" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="820" spans="2:2">
+    <row r="820" spans="1:2">
       <c r="B820" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="821" spans="2:2">
+    <row r="821" spans="1:2">
+      <c r="A821" t="s">
+        <v>885</v>
+      </c>
       <c r="B821" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="822" spans="2:2">
+    <row r="822" spans="1:2">
+      <c r="A822" t="s">
+        <v>885</v>
+      </c>
       <c r="B822" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="823" spans="2:2">
+    <row r="823" spans="1:2">
+      <c r="A823" t="s">
+        <v>887</v>
+      </c>
       <c r="B823" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="824" spans="2:2">
+    <row r="824" spans="1:2">
+      <c r="A824" t="s">
+        <v>885</v>
+      </c>
       <c r="B824" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="825" spans="2:2">
+    <row r="825" spans="1:2">
+      <c r="A825" t="s">
+        <v>885</v>
+      </c>
       <c r="B825" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="826" spans="2:2">
+    <row r="826" spans="1:2">
+      <c r="A826" t="s">
+        <v>885</v>
+      </c>
       <c r="B826" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="827" spans="2:2">
+    <row r="827" spans="1:2">
+      <c r="A827" t="s">
+        <v>885</v>
+      </c>
       <c r="B827" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="828" spans="2:2">
+    <row r="828" spans="1:2">
+      <c r="A828" t="s">
+        <v>885</v>
+      </c>
       <c r="B828" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="829" spans="2:2">
+    <row r="829" spans="1:2">
+      <c r="A829" t="s">
+        <v>885</v>
+      </c>
       <c r="B829" t="s">
         <v>750</v>
       </c>
     </row>
-    <row r="830" spans="2:2">
+    <row r="830" spans="1:2">
+      <c r="A830" t="s">
+        <v>885</v>
+      </c>
       <c r="B830" t="s">
         <v>860</v>
       </c>
     </row>
-    <row r="831" spans="2:2">
+    <row r="831" spans="1:2">
+      <c r="A831" t="s">
+        <v>885</v>
+      </c>
       <c r="B831" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="832" spans="2:2">
+    <row r="832" spans="1:2">
+      <c r="A832" t="s">
+        <v>885</v>
+      </c>
       <c r="B832" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="833" spans="2:2">
+    <row r="833" spans="1:2">
+      <c r="A833" t="s">
+        <v>885</v>
+      </c>
       <c r="B833" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="834" spans="2:2">
+    <row r="834" spans="1:2">
+      <c r="A834" t="s">
+        <v>885</v>
+      </c>
       <c r="B834" t="s">
         <v>822</v>
       </c>
     </row>
-    <row r="835" spans="2:2">
+    <row r="835" spans="1:2">
+      <c r="A835" t="s">
+        <v>885</v>
+      </c>
       <c r="B835" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="836" spans="2:2">
+    <row r="836" spans="1:2">
+      <c r="A836" t="s">
+        <v>885</v>
+      </c>
       <c r="B836" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="837" spans="2:2">
+    <row r="837" spans="1:2">
+      <c r="A837" t="s">
+        <v>885</v>
+      </c>
       <c r="B837" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="838" spans="2:2">
+    <row r="838" spans="1:2">
+      <c r="A838" t="s">
+        <v>885</v>
+      </c>
       <c r="B838" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="839" spans="2:2">
+    <row r="839" spans="1:2">
+      <c r="A839" t="s">
+        <v>885</v>
+      </c>
       <c r="B839" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="840" spans="2:2">
+    <row r="840" spans="1:2">
+      <c r="A840" t="s">
+        <v>885</v>
+      </c>
       <c r="B840" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="841" spans="2:2">
+    <row r="841" spans="1:2">
+      <c r="A841" t="s">
+        <v>885</v>
+      </c>
       <c r="B841" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="842" spans="2:2">
+    <row r="842" spans="1:2">
+      <c r="A842" t="s">
+        <v>885</v>
+      </c>
       <c r="B842" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="843" spans="2:2">
+    <row r="843" spans="1:2">
+      <c r="A843" t="s">
+        <v>885</v>
+      </c>
       <c r="B843" t="s">
         <v>811</v>
       </c>
     </row>
-    <row r="844" spans="2:2">
+    <row r="844" spans="1:2">
+      <c r="A844" t="s">
+        <v>885</v>
+      </c>
       <c r="B844" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="845" spans="2:2">
+    <row r="845" spans="1:2">
       <c r="B845" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="846" spans="2:2">
+    <row r="846" spans="1:2">
+      <c r="A846" t="s">
+        <v>885</v>
+      </c>
       <c r="B846" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="847" spans="2:2">
+    <row r="847" spans="1:2">
+      <c r="A847" t="s">
+        <v>885</v>
+      </c>
       <c r="B847" t="s">
         <v>765</v>
       </c>
     </row>
-    <row r="848" spans="2:2">
+    <row r="848" spans="1:2">
+      <c r="A848" t="s">
+        <v>885</v>
+      </c>
       <c r="B848" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="849" spans="2:2">
+    <row r="849" spans="1:2">
+      <c r="A849" t="s">
+        <v>885</v>
+      </c>
       <c r="B849" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="850" spans="2:2">
+    <row r="850" spans="1:2">
+      <c r="A850" t="s">
+        <v>885</v>
+      </c>
       <c r="B850" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="851" spans="2:2">
+    <row r="851" spans="1:2">
+      <c r="A851" t="s">
+        <v>885</v>
+      </c>
       <c r="B851" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="852" spans="2:2">
+    <row r="852" spans="1:2">
+      <c r="A852" t="s">
+        <v>885</v>
+      </c>
       <c r="B852" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="853" spans="2:2">
+    <row r="853" spans="1:2">
+      <c r="A853" t="s">
+        <v>885</v>
+      </c>
       <c r="B853" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="854" spans="2:2">
+    <row r="854" spans="1:2">
+      <c r="A854" t="s">
+        <v>885</v>
+      </c>
       <c r="B854" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="855" spans="2:2">
+    <row r="855" spans="1:2">
+      <c r="A855" t="s">
+        <v>885</v>
+      </c>
       <c r="B855" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="856" spans="2:2">
+    <row r="856" spans="1:2">
+      <c r="A856" t="s">
+        <v>885</v>
+      </c>
       <c r="B856" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="857" spans="2:2">
+    <row r="857" spans="1:2">
+      <c r="A857" t="s">
+        <v>887</v>
+      </c>
       <c r="B857" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="858" spans="2:2">
+    <row r="858" spans="1:2">
       <c r="B858" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="859" spans="2:2">
+    <row r="859" spans="1:2">
+      <c r="A859" t="s">
+        <v>885</v>
+      </c>
       <c r="B859" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="860" spans="2:2">
+    <row r="860" spans="1:2">
+      <c r="A860" t="s">
+        <v>885</v>
+      </c>
       <c r="B860" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="861" spans="2:2">
+    <row r="861" spans="1:2">
+      <c r="A861" t="s">
+        <v>885</v>
+      </c>
       <c r="B861" t="s">
         <v>713</v>
       </c>
     </row>
-    <row r="862" spans="2:2">
+    <row r="862" spans="1:2">
+      <c r="A862" t="s">
+        <v>885</v>
+      </c>
       <c r="B862" t="s">
         <v>751</v>
       </c>
     </row>
-    <row r="863" spans="2:2">
+    <row r="863" spans="1:2">
+      <c r="A863" t="s">
+        <v>887</v>
+      </c>
       <c r="B863" t="s">
         <v>845</v>
       </c>
     </row>
-    <row r="864" spans="2:2">
+    <row r="864" spans="1:2">
+      <c r="A864" t="s">
+        <v>887</v>
+      </c>
       <c r="B864" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="865" spans="2:2">
+    <row r="865" spans="1:2">
+      <c r="A865" t="s">
+        <v>885</v>
+      </c>
       <c r="B865" t="s">
         <v>884</v>
       </c>
     </row>
-    <row r="866" spans="2:2">
+    <row r="866" spans="1:2">
+      <c r="A866" t="s">
+        <v>885</v>
+      </c>
       <c r="B866" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="867" spans="2:2">
+    <row r="867" spans="1:2">
       <c r="B867" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="868" spans="2:2">
+    <row r="868" spans="1:2">
+      <c r="A868" t="s">
+        <v>887</v>
+      </c>
       <c r="B868" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="869" spans="2:2">
+    <row r="869" spans="1:2">
+      <c r="A869" t="s">
+        <v>885</v>
+      </c>
       <c r="B869" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="870" spans="2:2">
+    <row r="870" spans="1:2">
+      <c r="A870" t="s">
+        <v>885</v>
+      </c>
       <c r="B870" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="871" spans="2:2">
+    <row r="871" spans="1:2">
+      <c r="A871" t="s">
+        <v>885</v>
+      </c>
       <c r="B871" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="872" spans="2:2">
+    <row r="872" spans="1:2">
+      <c r="A872" t="s">
+        <v>885</v>
+      </c>
       <c r="B872" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="873" spans="2:2">
+    <row r="873" spans="1:2">
+      <c r="A873" t="s">
+        <v>885</v>
+      </c>
       <c r="B873" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="874" spans="2:2">
+    <row r="874" spans="1:2">
+      <c r="A874" t="s">
+        <v>885</v>
+      </c>
       <c r="B874" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="875" spans="2:2">
+    <row r="875" spans="1:2">
+      <c r="A875" t="s">
+        <v>885</v>
+      </c>
       <c r="B875" t="s">
         <v>766</v>
       </c>
     </row>
-    <row r="876" spans="2:2">
+    <row r="876" spans="1:2">
+      <c r="A876" t="s">
+        <v>885</v>
+      </c>
       <c r="B876" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="877" spans="2:2">
+    <row r="877" spans="1:2">
       <c r="B877" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="878" spans="2:2">
+    <row r="878" spans="1:2">
+      <c r="A878" t="s">
+        <v>885</v>
+      </c>
       <c r="B878" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="879" spans="2:2">
+    <row r="879" spans="1:2">
+      <c r="A879" t="s">
+        <v>885</v>
+      </c>
       <c r="B879" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="880" spans="2:2">
+    <row r="880" spans="1:2">
+      <c r="A880" t="s">
+        <v>885</v>
+      </c>
       <c r="B880" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="881" spans="2:2">
+    <row r="881" spans="1:2">
+      <c r="A881" t="s">
+        <v>885</v>
+      </c>
       <c r="B881" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="882" spans="2:2">
+    <row r="882" spans="1:2">
+      <c r="A882" t="s">
+        <v>885</v>
+      </c>
       <c r="B882" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="883" spans="2:2">
+    <row r="883" spans="1:2">
+      <c r="A883" t="s">
+        <v>887</v>
+      </c>
       <c r="B883" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="884" spans="2:2">
+    <row r="884" spans="1:2">
+      <c r="A884" t="s">
+        <v>885</v>
+      </c>
       <c r="B884" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="885" spans="2:2">
+    <row r="885" spans="1:2">
+      <c r="A885" t="s">
+        <v>885</v>
+      </c>
       <c r="B885" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="886" spans="2:2">
+    <row r="886" spans="1:2">
+      <c r="A886" t="s">
+        <v>885</v>
+      </c>
       <c r="B886" t="s">
         <v>604</v>
       </c>

</xml_diff>